<commit_message>
added models and untested changes
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E25DEA78-9EB0-43B2-AA3A-059DCD573D82}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50090292-4119-40B5-AAAB-B991EE0C23A2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -346,6 +346,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,22 +655,22 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="19" customWidth="1"/>
     <col min="3" max="3" width="10" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="20" customWidth="1"/>
     <col min="5" max="5" width="20" style="18" customWidth="1"/>
-    <col min="6" max="6" width="71.5546875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="72.33203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="71.5703125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="72.28515625" style="22" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -677,7 +681,7 @@
       <c r="F1"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="6"/>
       <c r="C2"/>
@@ -688,7 +692,7 @@
       <c r="F2"/>
       <c r="G2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -711,7 +715,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>45201</v>
       </c>
@@ -732,7 +736,13 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>45202</v>
+      </c>
+      <c r="B5" s="19">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="C5" s="14"/>
       <c r="D5" s="20" t="str">
         <f t="shared" si="0"/>
@@ -743,7 +753,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="14"/>
       <c r="D6" s="20" t="str">
         <f>IF(OR(B6=0, C6=0),"", C6-B6)</f>
@@ -754,7 +764,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="14"/>
       <c r="D7" s="20" t="str">
         <f t="shared" ref="D7:D30" si="1">IF(OR(B7=0, C7=0),"", C7-B7)</f>
@@ -765,7 +775,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -775,7 +785,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -785,7 +795,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -795,7 +805,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -805,7 +815,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -815,7 +825,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -825,7 +835,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -835,7 +845,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -845,7 +855,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -855,7 +865,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -865,7 +875,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -875,7 +885,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -885,7 +895,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -895,7 +905,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -905,7 +915,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -915,7 +925,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -925,7 +935,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -935,7 +945,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -945,7 +955,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -955,7 +965,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -965,7 +975,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -975,7 +985,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -985,7 +995,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30" s="20" t="str">
         <f t="shared" si="1"/>
         <v/>

</xml_diff>

<commit_message>
Lots of window progress
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C10F9B09-334D-4F59-9F9D-07A87D8E519F}"/>
+  <xr:revisionPtr revIDLastSave="429" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F791463E-0536-498A-A836-D0CDC051C249}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Start Time:</t>
   </si>
@@ -75,6 +97,51 @@
   </si>
   <si>
     <t>Make dragging the dividers change the size of the columns</t>
+  </si>
+  <si>
+    <t>Goal: 2+ hours weekdays 5+ hours weekends</t>
+  </si>
+  <si>
+    <t>Total Time:</t>
+  </si>
+  <si>
+    <t>Distance From Goal Time:</t>
+  </si>
+  <si>
+    <t>Running Goal:</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>4 hours</t>
+  </si>
+  <si>
+    <t>5 hours</t>
+  </si>
+  <si>
+    <t>6 hours</t>
+  </si>
+  <si>
+    <t>Goal Time:</t>
+  </si>
+  <si>
+    <t>8 hours</t>
+  </si>
+  <si>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>15 hours</t>
+  </si>
+  <si>
+    <t>20 hours</t>
+  </si>
+  <si>
+    <t>Got a lot of work on the GridPane component.</t>
+  </si>
+  <si>
+    <t>Refactor the ConversationWindow to have its state managed by the page. Also refactor it to have a toggle between 3.5 and 4.</t>
   </si>
 </sst>
 </file>
@@ -86,7 +153,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +168,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +221,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB061FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4A7FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAB81FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -315,14 +433,435 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79995117038483843"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79995117038483843"/>
+      </left>
+      <right style="thin">
+        <color theme="9" tint="0.79995117038483843"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -331,18 +870,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -355,12 +890,85 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFAB81FF"/>
+      <color rgb="FFC4A7FF"/>
+      <color rgb="FFB061FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -676,390 +1284,610 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="10" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="20" style="18" customWidth="1"/>
-    <col min="6" max="6" width="71.5546875" style="26" customWidth="1"/>
-    <col min="7" max="7" width="72.33203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="20" style="15" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="37" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="29"/>
+    <col min="12" max="15" width="32.7109375" style="30"/>
+    <col min="16" max="16" width="32.7109375" style="55"/>
+    <col min="17" max="17" width="32.7109375" style="60"/>
+    <col min="18" max="18" width="32.7109375" style="31"/>
+    <col min="19" max="16384" width="32.7109375" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1"/>
-      <c r="D1" s="8"/>
-      <c r="E1"/>
-      <c r="F1" s="23"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="6"/>
-      <c r="C2"/>
-      <c r="D2" s="8" t="s">
+      <c r="C1" s="5"/>
+      <c r="E1" s="7"/>
+      <c r="G1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="J1" s="32"/>
+    </row>
+    <row r="2" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2"/>
-      <c r="F2" s="23"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="22"/>
+      <c r="J2" s="32"/>
+    </row>
+    <row r="3" spans="1:18" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="G3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="I3"/>
+      <c r="J3" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="34">
         <v>45201</v>
       </c>
-      <c r="B4" s="12">
+      <c r="L3" s="34">
+        <v>45202</v>
+      </c>
+      <c r="M3" s="34">
+        <v>45203</v>
+      </c>
+      <c r="N3" s="34">
+        <v>45204</v>
+      </c>
+      <c r="O3" s="34">
+        <v>45205</v>
+      </c>
+      <c r="P3" s="50">
+        <v>45206</v>
+      </c>
+      <c r="Q3" s="50">
+        <v>45207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" s="26">
+        <v>45201</v>
+      </c>
+      <c r="C4" s="10">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C4" s="13">
+      <c r="D4" s="11">
         <v>0.52777777777777779</v>
       </c>
-      <c r="D4" s="20">
-        <f t="shared" ref="D4:D5" si="0">IF(OR(B4=0, C4=0),"", C4-B4)</f>
+      <c r="E4" s="17">
+        <f>IF(OR(C4=0, D4=0),"", D4-C4)</f>
         <v>6.9444444444444475E-2</v>
       </c>
-      <c r="E4" s="17" t="str">
-        <f>IF(D4="","",_xlfn.CONCAT(HOUR(SUM($D$4:D4))," hours ",MINUTE(SUM($D$4:D4))," minutes"))</f>
+      <c r="F4" s="14" t="str">
+        <f>IF(E4="","",_xlfn.CONCAT(HOUR(SUM($E$4:E4))," hours ",MINUTE(SUM($E$4:E4))," minutes"))</f>
         <v>1 hours 40 minutes</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+      <c r="G4" s="20"/>
+      <c r="H4" s="24"/>
+      <c r="I4"/>
+      <c r="J4" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="39" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, K$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>01 hours 40 minutes</v>
+      </c>
+      <c r="L4" s="39" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, L$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>02 hours 53 minutes</v>
+      </c>
+      <c r="M4" s="39" t="str">
+        <f t="shared" ref="M4:Q4" si="0">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, M$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>02 hours 20 minutes</v>
+      </c>
+      <c r="N4" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>02 hours 56 minutes</v>
+      </c>
+      <c r="O4" s="39" t="str">
+        <f t="shared" si="0"/>
+        <v>03 hours 52 minutes</v>
+      </c>
+      <c r="P4" s="49" t="str">
+        <f t="shared" si="0"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="Q4" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="R4" s="38"/>
+    </row>
+    <row r="5" spans="1:18" s="43" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5" s="27">
         <v>45202</v>
       </c>
-      <c r="B5" s="19">
+      <c r="C5" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C5" s="14">
+      <c r="D5" s="12">
         <v>0.82847222222222217</v>
       </c>
-      <c r="D5" s="20">
-        <f t="shared" si="0"/>
+      <c r="E5" s="17">
+        <f t="shared" ref="E5" si="1">IF(OR(C5=0, D5=0),"", D5-C5)</f>
         <v>0.1201388888888888</v>
       </c>
-      <c r="E5" s="18" t="str">
-        <f>IF(D5="","",_xlfn.CONCAT(HOUR(SUM($D$4:D5))," hours ",MINUTE(SUM($D$4:D5))," minutes"))</f>
+      <c r="F5" s="15" t="str">
+        <f>IF(E5="","",_xlfn.CONCAT(HOUR(SUM($E$4:E5))," hours ",MINUTE(SUM($E$4:E5))," minutes"))</f>
         <v>4 hours 33 minutes</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="G5" s="21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+      <c r="H5" s="25"/>
+      <c r="I5"/>
+      <c r="J5" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="54" t="str">
+        <f>IF(INT(LEFT(K$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(K$6,1)-SUM(LEFT(K$4, 2), (MID(K4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(K$6,1)-SUM(LEFT(K$4, 2), (MID(K4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>0 hours 20 minutes</v>
+      </c>
+      <c r="L5" s="43" t="str">
+        <f>IF(INT(LEFT(L$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(L$6,1)-SUM(LEFT(L$4, 2), (MID(L4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(L$6,1)-SUM(LEFT(L$4, 2), (MID(L4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>Goal Met!</v>
+      </c>
+      <c r="M5" s="52" t="str">
+        <f>IF(INT(LEFT(M$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(M$6,1)-SUM(LEFT(M$4, 2), (MID(M4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(M$6,1)-SUM(LEFT(M$4, 2), (MID(M4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>Goal Met!</v>
+      </c>
+      <c r="N5" s="43" t="str">
+        <f t="shared" ref="N5:Q5" si="2">IF(INT(LEFT(N$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>Goal Met!</v>
+      </c>
+      <c r="O5" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v>Goal Met!</v>
+      </c>
+      <c r="P5" s="57" t="str">
+        <f t="shared" si="2"/>
+        <v>5 hours 0 minutes</v>
+      </c>
+      <c r="Q5" s="58" t="str">
+        <f t="shared" si="2"/>
+        <v>5 hours 0 minutes</v>
+      </c>
+      <c r="R5" s="44"/>
+    </row>
+    <row r="6" spans="1:18" s="43" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6" s="27">
         <v>45203</v>
       </c>
-      <c r="B6" s="19">
+      <c r="C6" s="16">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C6" s="14">
+      <c r="D6" s="12">
         <v>0.50694444444444442</v>
       </c>
-      <c r="D6" s="20">
-        <f>IF(OR(B6=0, C6=0),"", C6-B6)</f>
+      <c r="E6" s="17">
+        <f>IF(OR(C6=0, D6=0),"", D6-C6)</f>
         <v>9.7222222222222154E-2</v>
       </c>
-      <c r="E6" s="18" t="str">
-        <f>IF(D6="","",_xlfn.CONCAT(HOUR(SUM($D$4:D6))," hours ",MINUTE(SUM($D$4:D6))," minutes"))</f>
+      <c r="F6" s="15" t="str">
+        <f>IF(E6="","",_xlfn.CONCAT(HOUR(SUM($E$4:E6))," hours ",MINUTE(SUM($E$4:E6))," minutes"))</f>
         <v>6 hours 53 minutes</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="G6" s="21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="H6" s="25"/>
+      <c r="I6"/>
+      <c r="J6" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="44"/>
+    </row>
+    <row r="7" spans="1:18" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7" s="27">
         <v>45204</v>
       </c>
-      <c r="B7" s="19">
+      <c r="C7" s="16">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C7" s="14">
+      <c r="D7" s="12">
         <v>0.5180555555555556</v>
       </c>
-      <c r="D7" s="20">
-        <f t="shared" ref="D7:D30" si="1">IF(OR(B7=0, C7=0),"", C7-B7)</f>
+      <c r="E7" s="17">
+        <f t="shared" ref="E7:E30" si="3">IF(OR(C7=0, D7=0),"", D7-C7)</f>
         <v>0.12222222222222229</v>
       </c>
-      <c r="E7" s="18" t="str">
-        <f>IF(D7="","",_xlfn.CONCAT(HOUR(SUM($D$4:D7))," hours ",MINUTE(SUM($D$4:D7))," minutes"))</f>
+      <c r="F7" s="15" t="str">
+        <f>IF(E7="","",_xlfn.CONCAT(HOUR(SUM($E$4:E7))," hours ",MINUTE(SUM($E$4:E7))," minutes"))</f>
         <v>9 hours 49 minutes</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="G7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E8" s="18" t="str">
-        <f>IF(D8="","",_xlfn.CONCAT(HOUR(SUM($D$4:D8))," hours ",MINUTE(SUM($D$4:D8))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E9" s="18" t="str">
-        <f>IF(D9="","",_xlfn.CONCAT(HOUR(SUM($D$4:D9))," hours ",MINUTE(SUM($D$4:D9))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E10" s="18" t="str">
-        <f>IF(D10="","",_xlfn.CONCAT(HOUR(SUM($D$4:D10))," hours ",MINUTE(SUM($D$4:D10))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E11" s="18" t="str">
-        <f>IF(D11="","",_xlfn.CONCAT(HOUR(SUM($D$4:D11))," hours ",MINUTE(SUM($D$4:D11))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E12" s="18" t="str">
-        <f>IF(D12="","",_xlfn.CONCAT(HOUR(SUM($D$4:D12))," hours ",MINUTE(SUM($D$4:D12))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E13" s="18" t="str">
-        <f>IF(D13="","",_xlfn.CONCAT(HOUR(SUM($D$4:D13))," hours ",MINUTE(SUM($D$4:D13))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E14" s="18" t="str">
-        <f>IF(D14="","",_xlfn.CONCAT(HOUR(SUM($D$4:D14))," hours ",MINUTE(SUM($D$4:D14))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E15" s="18" t="str">
-        <f>IF(D15="","",_xlfn.CONCAT(HOUR(SUM($D$4:D15))," hours ",MINUTE(SUM($D$4:D15))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E16" s="18" t="str">
-        <f>IF(D16="","",_xlfn.CONCAT(HOUR(SUM($D$4:D16))," hours ",MINUTE(SUM($D$4:D16))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E17" s="18" t="str">
-        <f>IF(D17="","",_xlfn.CONCAT(HOUR(SUM($D$4:D17))," hours ",MINUTE(SUM($D$4:D17))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E18" s="18" t="str">
-        <f>IF(D18="","",_xlfn.CONCAT(HOUR(SUM($D$4:D18))," hours ",MINUTE(SUM($D$4:D18))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E19" s="18" t="str">
-        <f>IF(D19="","",_xlfn.CONCAT(HOUR(SUM($D$4:D19))," hours ",MINUTE(SUM($D$4:D19))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E20" s="18" t="str">
-        <f>IF(D20="","",_xlfn.CONCAT(HOUR(SUM($D$4:D20))," hours ",MINUTE(SUM($D$4:D20))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E21" s="18" t="str">
-        <f>IF(D21="","",_xlfn.CONCAT(HOUR(SUM($D$4:D21))," hours ",MINUTE(SUM($D$4:D21))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E22" s="18" t="str">
-        <f>IF(D22="","",_xlfn.CONCAT(HOUR(SUM($D$4:D22))," hours ",MINUTE(SUM($D$4:D22))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D23" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E23" s="18" t="str">
-        <f>IF(D23="","",_xlfn.CONCAT(HOUR(SUM($D$4:D23))," hours ",MINUTE(SUM($D$4:D23))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D24" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E24" s="18" t="str">
-        <f>IF(D24="","",_xlfn.CONCAT(HOUR(SUM($D$4:D24))," hours ",MINUTE(SUM($D$4:D24))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D25" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E25" s="18" t="str">
-        <f>IF(D25="","",_xlfn.CONCAT(HOUR(SUM($D$4:D25))," hours ",MINUTE(SUM($D$4:D25))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D26" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E26" s="18" t="str">
-        <f>IF(D26="","",_xlfn.CONCAT(HOUR(SUM($D$4:D26))," hours ",MINUTE(SUM($D$4:D26))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D27" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E27" s="18" t="str">
-        <f>IF(D27="","",_xlfn.CONCAT(HOUR(SUM($D$4:D27))," hours ",MINUTE(SUM($D$4:D27))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D28" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E28" s="18" t="str">
-        <f>IF(D28="","",_xlfn.CONCAT(HOUR(SUM($D$4:D28))," hours ",MINUTE(SUM($D$4:D28))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D29" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E29" s="18" t="str">
-        <f>IF(D29="","",_xlfn.CONCAT(HOUR(SUM($D$4:D29))," hours ",MINUTE(SUM($D$4:D29))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D30" s="20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E30" s="18" t="str">
-        <f>IF(D30="","",_xlfn.CONCAT(HOUR(SUM($D$4:D30))," hours ",MINUTE(SUM($D$4:D30))," minutes"))</f>
+      <c r="I7"/>
+      <c r="J7" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="61" t="str" cm="1">
+        <f t="array" ref="K7">INT((SUM(SUM(INT(LEFT($K$4:K$4, 2))), SUM(MID($K$4:K$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:K$4, 2))), SUM(MID($K$4:K$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>1 hours 40 minutes</v>
+      </c>
+      <c r="L7" s="43" t="str" cm="1">
+        <f t="array" ref="L7">INT((SUM(SUM(INT(LEFT($K$4:L$4, 2))), SUM(MID($K$4:L$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:L$4, 2))), SUM(MID($K$4:L$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>4 hours 33 minutes</v>
+      </c>
+      <c r="M7" s="43" t="str" cm="1">
+        <f t="array" ref="M7">INT((SUM(SUM(INT(LEFT($K$4:M$4, 2))), SUM(MID($K$4:M$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:M$4, 2))), SUM(MID($K$4:M$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>6 hours 53 minutes</v>
+      </c>
+      <c r="N7" s="43" t="str" cm="1">
+        <f t="array" ref="N7">INT((SUM(SUM(INT(LEFT($K$4:N$4, 2))), SUM(MID($K$4:N$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:N$4, 2))), SUM(MID($K$4:N$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>9 hours 49 minutes</v>
+      </c>
+      <c r="O7" s="62" t="str" cm="1">
+        <f t="array" ref="O7">INT((SUM(SUM(INT(LEFT($K$4:O$4, 2))), SUM(MID($K$4:O$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:O$4, 2))), SUM(MID($K$4:O$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>13 hours 41 minutes</v>
+      </c>
+      <c r="P7" s="63" t="str" cm="1">
+        <f t="array" ref="P7">INT((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>13 hours 41 minutes</v>
+      </c>
+      <c r="Q7" s="64" t="str" cm="1">
+        <f t="array" ref="Q7">INT((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>13 hours 41 minutes</v>
+      </c>
+      <c r="R7" s="48"/>
+    </row>
+    <row r="8" spans="1:18" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+      <c r="B8" s="27">
+        <v>45205</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0.52986111111111112</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="3"/>
+        <v>0.16111111111111109</v>
+      </c>
+      <c r="F8" s="15" t="str">
+        <f>IF(E8="","",_xlfn.CONCAT(HOUR(SUM($E$4:E8))," hours ",MINUTE(SUM($E$4:E8))," minutes"))</f>
+        <v>13 hours 41 minutes</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="R8" s="48"/>
+    </row>
+    <row r="9" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F9" s="15" t="str">
+        <f>IF(E9="","",_xlfn.CONCAT(HOUR(SUM($E$4:E9))," hours ",MINUTE(SUM($E$4:E9))," minutes"))</f>
+        <v/>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="25"/>
+      <c r="I9"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="45"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="40"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E10" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F10" s="15" t="str">
+        <f>IF(E10="","",_xlfn.CONCAT(HOUR(SUM($E$4:E10))," hours ",MINUTE(SUM($E$4:E10))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E11" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F11" s="15" t="str">
+        <f>IF(E11="","",_xlfn.CONCAT(HOUR(SUM($E$4:E11))," hours ",MINUTE(SUM($E$4:E11))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F12" s="15" t="str">
+        <f>IF(E12="","",_xlfn.CONCAT(HOUR(SUM($E$4:E12))," hours ",MINUTE(SUM($E$4:E12))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E13" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F13" s="15" t="str">
+        <f>IF(E13="","",_xlfn.CONCAT(HOUR(SUM($E$4:E13))," hours ",MINUTE(SUM($E$4:E13))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E14" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F14" s="15" t="str">
+        <f>IF(E14="","",_xlfn.CONCAT(HOUR(SUM($E$4:E14))," hours ",MINUTE(SUM($E$4:E14))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E15" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F15" s="15" t="str">
+        <f>IF(E15="","",_xlfn.CONCAT(HOUR(SUM($E$4:E15))," hours ",MINUTE(SUM($E$4:E15))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E16" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F16" s="15" t="str">
+        <f>IF(E16="","",_xlfn.CONCAT(HOUR(SUM($E$4:E16))," hours ",MINUTE(SUM($E$4:E16))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F17" s="15" t="str">
+        <f>IF(E17="","",_xlfn.CONCAT(HOUR(SUM($E$4:E17))," hours ",MINUTE(SUM($E$4:E17))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F18" s="15" t="str">
+        <f>IF(E18="","",_xlfn.CONCAT(HOUR(SUM($E$4:E18))," hours ",MINUTE(SUM($E$4:E18))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F19" s="15" t="str">
+        <f>IF(E19="","",_xlfn.CONCAT(HOUR(SUM($E$4:E19))," hours ",MINUTE(SUM($E$4:E19))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F20" s="15" t="str">
+        <f>IF(E20="","",_xlfn.CONCAT(HOUR(SUM($E$4:E20))," hours ",MINUTE(SUM($E$4:E20))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F21" s="15" t="str">
+        <f>IF(E21="","",_xlfn.CONCAT(HOUR(SUM($E$4:E21))," hours ",MINUTE(SUM($E$4:E21))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F22" s="15" t="str">
+        <f>IF(E22="","",_xlfn.CONCAT(HOUR(SUM($E$4:E22))," hours ",MINUTE(SUM($E$4:E22))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F23" s="15" t="str">
+        <f>IF(E23="","",_xlfn.CONCAT(HOUR(SUM($E$4:E23))," hours ",MINUTE(SUM($E$4:E23))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F24" s="15" t="str">
+        <f>IF(E24="","",_xlfn.CONCAT(HOUR(SUM($E$4:E24))," hours ",MINUTE(SUM($E$4:E24))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F25" s="15" t="str">
+        <f>IF(E25="","",_xlfn.CONCAT(HOUR(SUM($E$4:E25))," hours ",MINUTE(SUM($E$4:E25))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F26" s="15" t="str">
+        <f>IF(E26="","",_xlfn.CONCAT(HOUR(SUM($E$4:E26))," hours ",MINUTE(SUM($E$4:E26))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F27" s="15" t="str">
+        <f>IF(E27="","",_xlfn.CONCAT(HOUR(SUM($E$4:E27))," hours ",MINUTE(SUM($E$4:E27))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F28" s="15" t="str">
+        <f>IF(E28="","",_xlfn.CONCAT(HOUR(SUM($E$4:E28))," hours ",MINUTE(SUM($E$4:E28))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F29" s="15" t="str">
+        <f>IF(E29="","",_xlfn.CONCAT(HOUR(SUM($E$4:E29))," hours ",MINUTE(SUM($E$4:E29))," minutes"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="F30" s="15" t="str">
+        <f>IF(E30="","",_xlfn.CONCAT(HOUR(SUM($E$4:E30))," hours ",MINUTE(SUM($E$4:E30))," minutes"))</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Got themes set up and more
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F791463E-0536-498A-A836-D0CDC051C249}"/>
+  <xr:revisionPtr revIDLastSave="437" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E51DA13-8BF7-40E3-953F-0CA04905B81E}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Start Time:</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Refactor the ConversationWindow to have its state managed by the page. Also refactor it to have a toggle between 3.5 and 4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Got themes set up, added GPT switch to conversation window, added styles accordingly, got a landing page and sign in/up started</t>
+  </si>
+  <si>
+    <t>Get conversation window talking to the backend. More work on the editor page</t>
   </si>
 </sst>
 </file>
@@ -1286,8 +1292,8 @@
   </sheetPr>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1434,7 @@
       </c>
       <c r="P4" s="49" t="str">
         <f t="shared" si="0"/>
-        <v>00 hours 00 minutes</v>
+        <v>04 hours 18 minutes</v>
       </c>
       <c r="Q4" s="51" t="str">
         <f t="shared" si="0"/>
@@ -1484,11 +1490,11 @@
         <v>Goal Met!</v>
       </c>
       <c r="P5" s="57" t="str">
-        <f t="shared" si="2"/>
-        <v>5 hours 0 minutes</v>
+        <f>IF(INT(LEFT(P$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(P$6,1)-SUM(LEFT(P$4, 2), (MID(P4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(P$6,1)-SUM(LEFT(P$4, 2), (MID(P4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>1 hours 42 minutes</v>
       </c>
       <c r="Q5" s="58" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(INT(LEFT(Q$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>5 hours 0 minutes</v>
       </c>
       <c r="R5" s="44"/>
@@ -1594,11 +1600,11 @@
       </c>
       <c r="P7" s="63" t="str" cm="1">
         <f t="array" ref="P7">INT((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>13 hours 41 minutes</v>
+        <v>17 hours 59 minutes</v>
       </c>
       <c r="Q7" s="64" t="str" cm="1">
         <f t="array" ref="Q7">INT((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>13 hours 41 minutes</v>
+        <v>17 hours 59 minutes</v>
       </c>
       <c r="R7" s="48"/>
     </row>
@@ -1654,21 +1660,31 @@
       </c>
       <c r="R8" s="48"/>
     </row>
-    <row r="9" spans="1:18" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A9"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="B9" s="27">
+        <v>45206</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="3"/>
+        <v>0.1791666666666667</v>
       </c>
       <c r="F9" s="15" t="str">
         <f>IF(E9="","",_xlfn.CONCAT(HOUR(SUM($E$4:E9))," hours ",MINUTE(SUM($E$4:E9))," minutes"))</f>
-        <v/>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="25"/>
+        <v>17 hours 59 minutes</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="I9"/>
       <c r="J9" s="37"/>
       <c r="K9" s="45"/>

</xml_diff>

<commit_message>
Frontend chat component hits GPT!! +more
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="444" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DD83D0C-4D02-488E-B632-7DE9C55B0DF5}"/>
+  <xr:revisionPtr revIDLastSave="457" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C20D1582-8908-4861-BCE0-72058B0F912A}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Start Time:</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>I didn't get the ConversationWindow tied to GPT yet. Do that</t>
+  </si>
+  <si>
+    <t>Frontend conversationWindow hits GPT! Also the TextField is multiline now</t>
+  </si>
+  <si>
+    <t>I need to start work on the syntax code display. I don't want code to be shown the same as regular messages. Fix the fact that multiline messages don't actually appear multiline in messages</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1305,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1450,7 @@
       </c>
       <c r="Q4" s="51" t="str">
         <f t="shared" si="0"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 25 minutes</v>
       </c>
       <c r="R4" s="38"/>
     </row>
@@ -1501,7 +1507,7 @@
       </c>
       <c r="Q5" s="58" t="str">
         <f>IF(INT(LEFT(Q$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>5 hours 0 minutes</v>
+        <v>4 hours 35 minutes</v>
       </c>
       <c r="R5" s="44"/>
     </row>
@@ -1610,7 +1616,7 @@
       </c>
       <c r="Q7" s="64" t="str" cm="1">
         <f t="array" ref="Q7">INT((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>20 hours 9 minutes</v>
+        <v>21 hours 34 minutes</v>
       </c>
       <c r="R7" s="48"/>
     </row>
@@ -1723,14 +1729,29 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E11" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+    <row r="11" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="27">
+        <v>45207</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0.46875</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E11" s="17">
+        <f>IF(OR(C11=0, D11=0),"", D11-C11)</f>
+        <v>5.902777777777779E-2</v>
       </c>
       <c r="F11" s="15" t="str">
         <f>IF(E11="","",_xlfn.CONCAT(HOUR(SUM($E$4:E11))," hours ",MINUTE(SUM($E$4:E11))," minutes"))</f>
-        <v/>
+        <v>21 hours 34 minutes</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code snippets now exist in chat
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="457" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C20D1582-8908-4861-BCE0-72058B0F912A}"/>
+  <xr:revisionPtr revIDLastSave="461" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7786A61-8900-4608-AFA8-CCC394386D12}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1304,8 +1304,8 @@
   </sheetPr>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,6 +1755,13 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="27">
+        <v>45207</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0.84375</v>
+      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>

</xml_diff>

<commit_message>
styled monaco, fixed code gen maybe
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="461" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7786A61-8900-4608-AFA8-CCC394386D12}"/>
+  <xr:revisionPtr revIDLastSave="525" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AB43DF4-9CFA-4575-BA1A-E23E9F5AC845}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Start Time:</t>
   </si>
@@ -160,6 +160,75 @@
   </si>
   <si>
     <t>I need to start work on the syntax code display. I don't want code to be shown the same as regular messages. Fix the fact that multiline messages don't actually appear multiline in messages</t>
+  </si>
+  <si>
+    <t>Got code snippets working in gpt messages</t>
+  </si>
+  <si>
+    <t>Next frontend task is the text editor. It's time to start slate stuff. Generally lots of frontend stuff needs doing. Maybe mock out layouts.</t>
+  </si>
+  <si>
+    <t>22 hours</t>
+  </si>
+  <si>
+    <t>24 hours</t>
+  </si>
+  <si>
+    <t>26 hours</t>
+  </si>
+  <si>
+    <t>28 hours</t>
+  </si>
+  <si>
+    <t>30 hours</t>
+  </si>
+  <si>
+    <t>35 hours</t>
+  </si>
+  <si>
+    <t>40 hours</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/@monaco-editor/react</t>
+  </si>
+  <si>
+    <t>Researching Web Containers and editors</t>
+  </si>
+  <si>
+    <t>Styled Monaco and researched a react preview solution. Pondered an easier solution than web containers, but I've decided against that for a better capstone</t>
+  </si>
+  <si>
+    <t>Setup Web containers: https://stackblitz.com/edit/stackblitz-webcontainer-api-starter-1ceghg?file=files.js https://webcontainers.io/tutorial/1-build-your-first-webcontainer-app</t>
+  </si>
+  <si>
+    <t>42 hours</t>
+  </si>
+  <si>
+    <t>44 hours</t>
+  </si>
+  <si>
+    <t>46 hours</t>
+  </si>
+  <si>
+    <t>48 hours</t>
+  </si>
+  <si>
+    <t>50 hours</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>55 hours</t>
+  </si>
+  <si>
+    <t>60 hours</t>
   </si>
 </sst>
 </file>
@@ -171,7 +240,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +272,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="46">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -482,7 +559,22 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color rgb="FFCCCCFF"/>
@@ -494,78 +586,48 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color rgb="FFCCCCFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FFCCCCFF"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFCCCCFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      </left>
       <right style="thin">
         <color rgb="FFCCCCFF"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFCCCCFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FFCCCCFF"/>
@@ -579,9 +641,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
       <right style="thin">
-        <color rgb="FFCCCCFF"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
@@ -591,25 +655,14 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color rgb="FFCCCCFF"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,97 +675,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCCCCFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFCCCCFF"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -749,34 +711,6 @@
         <color theme="9" tint="0.79998168889431442"/>
       </right>
       <top style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCFF"/>
-      </left>
-      <right style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -797,59 +731,31 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.79995117038483843"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.79998168889431442"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="9" tint="0.79995117038483843"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -873,11 +779,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCFF"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -923,58 +845,59 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1302,10 +1225,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,16 +1242,11 @@
     <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
     <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="37" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" style="29"/>
-    <col min="12" max="15" width="32.7109375" style="30"/>
-    <col min="16" max="16" width="32.7109375" style="55"/>
-    <col min="17" max="17" width="32.7109375" style="60"/>
-    <col min="18" max="18" width="32.7109375" style="31"/>
-    <col min="19" max="16384" width="32.7109375" style="30"/>
+    <col min="10" max="10" width="14.5703125" style="53" customWidth="1"/>
+    <col min="11" max="16384" width="32.7109375" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1338,9 +1256,9 @@
         <v>13</v>
       </c>
       <c r="H1" s="22"/>
-      <c r="J1" s="32"/>
-    </row>
-    <row r="2" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="E2" s="7" t="s">
@@ -1348,9 +1266,19 @@
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="22"/>
-      <c r="J2" s="32"/>
-    </row>
-    <row r="3" spans="1:18" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="29"/>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="54"/>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1374,32 +1302,74 @@
         <v>8</v>
       </c>
       <c r="I3"/>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="34">
+      <c r="K3" s="31">
         <v>45201</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="31">
         <v>45202</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="31">
         <v>45203</v>
       </c>
-      <c r="N3" s="34">
+      <c r="N3" s="31">
         <v>45204</v>
       </c>
-      <c r="O3" s="34">
+      <c r="O3" s="31">
         <v>45205</v>
       </c>
-      <c r="P3" s="50">
+      <c r="P3" s="41">
         <v>45206</v>
       </c>
-      <c r="Q3" s="50">
+      <c r="Q3" s="41">
         <v>45207</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="31">
+        <v>45208</v>
+      </c>
+      <c r="S3" s="31">
+        <v>45209</v>
+      </c>
+      <c r="T3" s="31">
+        <v>45210</v>
+      </c>
+      <c r="U3" s="31">
+        <v>45211</v>
+      </c>
+      <c r="V3" s="31">
+        <v>45212</v>
+      </c>
+      <c r="W3" s="41">
+        <v>45213</v>
+      </c>
+      <c r="X3" s="41">
+        <v>45214</v>
+      </c>
+      <c r="Y3" s="31">
+        <v>45215</v>
+      </c>
+      <c r="Z3" s="31">
+        <v>45216</v>
+      </c>
+      <c r="AA3" s="31">
+        <v>45217</v>
+      </c>
+      <c r="AB3" s="31">
+        <v>45218</v>
+      </c>
+      <c r="AC3" s="31">
+        <v>45219</v>
+      </c>
+      <c r="AD3" s="41">
+        <v>45220</v>
+      </c>
+      <c r="AE3" s="41">
+        <v>45221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -1421,40 +1391,95 @@
       <c r="G4" s="20"/>
       <c r="H4" s="24"/>
       <c r="I4"/>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="39" t="str">
+      <c r="K4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, K$3), "hh ""hours ""mm ""minutes""")</f>
         <v>01 hours 40 minutes</v>
       </c>
-      <c r="L4" s="39" t="str">
+      <c r="L4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, L$3), "hh ""hours ""mm ""minutes""")</f>
         <v>02 hours 53 minutes</v>
       </c>
-      <c r="M4" s="39" t="str">
+      <c r="M4" s="35" t="str">
         <f t="shared" ref="M4:Q4" si="0">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, M$3), "hh ""hours ""mm ""minutes""")</f>
         <v>02 hours 20 minutes</v>
       </c>
-      <c r="N4" s="39" t="str">
+      <c r="N4" s="35" t="str">
         <f t="shared" si="0"/>
         <v>02 hours 56 minutes</v>
       </c>
-      <c r="O4" s="39" t="str">
+      <c r="O4" s="35" t="str">
         <f t="shared" si="0"/>
         <v>03 hours 52 minutes</v>
       </c>
-      <c r="P4" s="49" t="str">
+      <c r="P4" s="40" t="str">
         <f t="shared" si="0"/>
         <v>06 hours 28 minutes</v>
       </c>
-      <c r="Q4" s="51" t="str">
+      <c r="Q4" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>01 hours 25 minutes</v>
-      </c>
-      <c r="R4" s="38"/>
-    </row>
-    <row r="5" spans="1:18" s="43" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>02 hours 38 minutes</v>
+      </c>
+      <c r="R4" s="35" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, R$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>03 hours 33 minutes</v>
+      </c>
+      <c r="S4" s="35" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, S$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="T4" s="35" t="str">
+        <f t="shared" ref="T4:X4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, T$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="U4" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="V4" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="W4" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="X4" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="Y4" s="35" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Y$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="Z4" s="35" t="str">
+        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Z$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AA4" s="35" t="str">
+        <f t="shared" ref="AA4:AE4" si="2">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AA$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AB4" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AC4" s="35" t="str">
+        <f t="shared" si="2"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AD4" s="40" t="str">
+        <f t="shared" si="2"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AE4" s="42" t="str">
+        <f t="shared" si="2"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -1466,7 +1491,7 @@
         <v>0.82847222222222217</v>
       </c>
       <c r="E5" s="17">
-        <f t="shared" ref="E5" si="1">IF(OR(C5=0, D5=0),"", D5-C5)</f>
+        <f t="shared" ref="E5" si="3">IF(OR(C5=0, D5=0),"", D5-C5)</f>
         <v>0.1201388888888888</v>
       </c>
       <c r="F5" s="15" t="str">
@@ -1478,40 +1503,95 @@
       </c>
       <c r="H5" s="25"/>
       <c r="I5"/>
-      <c r="J5" s="36" t="s">
+      <c r="J5" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="54" t="str">
+      <c r="K5" s="45" t="str">
         <f>IF(INT(LEFT(K$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(K$6,1)-SUM(LEFT(K$4, 2), (MID(K4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(K$6,1)-SUM(LEFT(K$4, 2), (MID(K4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>0 hours 20 minutes</v>
       </c>
-      <c r="L5" s="43" t="str">
+      <c r="L5" s="37" t="str">
         <f>IF(INT(LEFT(L$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(L$6,1)-SUM(LEFT(L$4, 2), (MID(L4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(L$6,1)-SUM(LEFT(L$4, 2), (MID(L4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>Goal Met!</v>
       </c>
-      <c r="M5" s="52" t="str">
+      <c r="M5" s="43" t="str">
         <f>IF(INT(LEFT(M$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(M$6,1)-SUM(LEFT(M$4, 2), (MID(M4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(M$6,1)-SUM(LEFT(M$4, 2), (MID(M4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>Goal Met!</v>
       </c>
-      <c r="N5" s="43" t="str">
-        <f t="shared" ref="N5:O5" si="2">IF(INT(LEFT(N$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+      <c r="N5" s="37" t="str">
+        <f t="shared" ref="N5:O5" si="4">IF(INT(LEFT(N$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(N$6,1)-SUM(LEFT(N$4, 2), (MID(N4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>Goal Met!</v>
       </c>
-      <c r="O5" s="43" t="str">
-        <f t="shared" si="2"/>
+      <c r="O5" s="37" t="str">
+        <f t="shared" si="4"/>
         <v>Goal Met!</v>
       </c>
-      <c r="P5" s="57" t="str">
+      <c r="P5" s="46" t="str">
         <f>IF(INT(LEFT(P$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(P$6,1)-SUM(LEFT(P$4, 2), (MID(P4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(P$6,1)-SUM(LEFT(P$4, 2), (MID(P4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
         <v>Goal Met!</v>
       </c>
-      <c r="Q5" s="58" t="str">
+      <c r="Q5" s="47" t="str">
         <f>IF(INT(LEFT(Q$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Q$6,1)-SUM(LEFT(Q$4, 2), (MID(Q4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>4 hours 35 minutes</v>
-      </c>
-      <c r="R5" s="44"/>
-    </row>
-    <row r="6" spans="1:18" s="43" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>2 hours 22 minutes</v>
+      </c>
+      <c r="R5" s="45" t="str">
+        <f>IF(INT(LEFT(R$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(R$6,1)-SUM(LEFT(R$4, 2), (MID(R4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(R$6,1)-SUM(LEFT(R$4, 2), (MID(R4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>Goal Met!</v>
+      </c>
+      <c r="S5" s="37" t="str">
+        <f>IF(INT(LEFT(S$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(S$6,1)-SUM(LEFT(S$4, 2), (MID(S4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(S$6,1)-SUM(LEFT(S$4, 2), (MID(S4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="T5" s="43" t="str">
+        <f>IF(INT(LEFT(T$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(T$6,1)-SUM(LEFT(T$4, 2), (MID(T4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(T$6,1)-SUM(LEFT(T$4, 2), (MID(T4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="U5" s="37" t="str">
+        <f t="shared" ref="U5:V5" si="5">IF(INT(LEFT(U$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="V5" s="37" t="str">
+        <f t="shared" si="5"/>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="W5" s="46" t="str">
+        <f>IF(INT(LEFT(W$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>5 hours 0 minutes</v>
+      </c>
+      <c r="X5" s="47" t="str">
+        <f>IF(INT(LEFT(X$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(X$6,1)-SUM(LEFT(X$4, 2), (MID(X4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(X$6,1)-SUM(LEFT(X$4, 2), (MID(X4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>5 hours 0 minutes</v>
+      </c>
+      <c r="Y5" s="45" t="str">
+        <f>IF(INT(LEFT(Y$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(Y$6,1)-SUM(LEFT(Y$4, 2), (MID(Y4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Y$6,1)-SUM(LEFT(Y$4, 2), (MID(Y4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="Z5" s="37" t="str">
+        <f>IF(INT(LEFT(Z$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="AA5" s="43" t="str">
+        <f>IF(INT(LEFT(AA$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(AA$6,1)-SUM(LEFT(AA$4, 2), (MID(AA4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AA$6,1)-SUM(LEFT(AA$4, 2), (MID(AA4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="AB5" s="37" t="str">
+        <f t="shared" ref="AB5:AC5" si="6">IF(INT(LEFT(AB$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(AB$6,1)-SUM(LEFT(AB$4, 2), (MID(AB4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AB$6,1)-SUM(LEFT(AB$4, 2), (MID(AB4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="AC5" s="37" t="str">
+        <f t="shared" si="6"/>
+        <v>2 hours 0 minutes</v>
+      </c>
+      <c r="AD5" s="46" t="str">
+        <f>IF(INT(LEFT(AD$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(AD$6,1)-SUM(LEFT(AD$4, 2), (MID(AD4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AD$6,1)-SUM(LEFT(AD$4, 2), (MID(AD4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>5 hours 0 minutes</v>
+      </c>
+      <c r="AE5" s="47" t="str">
+        <f>IF(INT(LEFT(AE$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(AE$6,1)-SUM(LEFT(AE$4, 2), (MID(AE4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AE$6,1)-SUM(LEFT(AE$4, 2), (MID(AE4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
+        <v>5 hours 0 minutes</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -1535,33 +1615,74 @@
       </c>
       <c r="H6" s="25"/>
       <c r="I6"/>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="43" t="s">
+      <c r="L6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="43" t="s">
+      <c r="N6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="43" t="s">
+      <c r="O6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="57" t="s">
+      <c r="P6" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="58" t="s">
+      <c r="Q6" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="44"/>
-    </row>
-    <row r="7" spans="1:18" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="R6" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y6" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD6" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE6" s="47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -1573,7 +1694,7 @@
         <v>0.5180555555555556</v>
       </c>
       <c r="E7" s="17">
-        <f t="shared" ref="E7:E30" si="3">IF(OR(C7=0, D7=0),"", D7-C7)</f>
+        <f t="shared" ref="E7:E30" si="7">IF(OR(C7=0, D7=0),"", D7-C7)</f>
         <v>0.12222222222222229</v>
       </c>
       <c r="F7" s="15" t="str">
@@ -1587,40 +1708,95 @@
         <v>12</v>
       </c>
       <c r="I7"/>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="61" t="str" cm="1">
+      <c r="K7" s="48" t="str" cm="1">
         <f t="array" ref="K7">INT((SUM(SUM(INT(LEFT($K$4:K$4, 2))), SUM(MID($K$4:K$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:K$4, 2))), SUM(MID($K$4:K$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>1 hours 40 minutes</v>
       </c>
-      <c r="L7" s="43" t="str" cm="1">
+      <c r="L7" s="37" t="str" cm="1">
         <f t="array" ref="L7">INT((SUM(SUM(INT(LEFT($K$4:L$4, 2))), SUM(MID($K$4:L$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:L$4, 2))), SUM(MID($K$4:L$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>4 hours 33 minutes</v>
       </c>
-      <c r="M7" s="43" t="str" cm="1">
+      <c r="M7" s="37" t="str" cm="1">
         <f t="array" ref="M7">INT((SUM(SUM(INT(LEFT($K$4:M$4, 2))), SUM(MID($K$4:M$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:M$4, 2))), SUM(MID($K$4:M$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>6 hours 53 minutes</v>
       </c>
-      <c r="N7" s="43" t="str" cm="1">
+      <c r="N7" s="37" t="str" cm="1">
         <f t="array" ref="N7">INT((SUM(SUM(INT(LEFT($K$4:N$4, 2))), SUM(MID($K$4:N$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:N$4, 2))), SUM(MID($K$4:N$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>9 hours 49 minutes</v>
       </c>
-      <c r="O7" s="62" t="str" cm="1">
+      <c r="O7" s="49" t="str" cm="1">
         <f t="array" ref="O7">INT((SUM(SUM(INT(LEFT($K$4:O$4, 2))), SUM(MID($K$4:O$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:O$4, 2))), SUM(MID($K$4:O$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>13 hours 41 minutes</v>
       </c>
-      <c r="P7" s="63" t="str" cm="1">
+      <c r="P7" s="50" t="str" cm="1">
         <f t="array" ref="P7">INT((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:P$4, 2))), SUM(MID($K$4:P$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
         <v>20 hours 9 minutes</v>
       </c>
-      <c r="Q7" s="64" t="str" cm="1">
+      <c r="Q7" s="51" t="str" cm="1">
         <f t="array" ref="Q7">INT((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Q$4, 2))), SUM(MID($K$4:Q$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>21 hours 34 minutes</v>
-      </c>
-      <c r="R7" s="48"/>
-    </row>
-    <row r="8" spans="1:18" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>22 hours 47 minutes</v>
+      </c>
+      <c r="R7" s="48" t="str" cm="1">
+        <f t="array" ref="R7">INT((SUM(SUM(INT(LEFT($K$4:R$4, 2))), SUM(MID($K$4:R$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:R$4, 2))), SUM(MID($K$4:R$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="S7" s="37" t="str" cm="1">
+        <f t="array" ref="S7">INT((SUM(SUM(INT(LEFT($K$4:S$4, 2))), SUM(MID($K$4:S$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:S$4, 2))), SUM(MID($K$4:S$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="T7" s="37" t="str" cm="1">
+        <f t="array" ref="T7">INT((SUM(SUM(INT(LEFT($K$4:T$4, 2))), SUM(MID($K$4:T$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:T$4, 2))), SUM(MID($K$4:T$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="U7" s="37" t="str" cm="1">
+        <f t="array" ref="U7">INT((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="V7" s="49" t="str" cm="1">
+        <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="W7" s="50" t="str" cm="1">
+        <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="X7" s="51" t="str" cm="1">
+        <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="Y7" s="48" t="str" cm="1">
+        <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="Z7" s="37" t="str" cm="1">
+        <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="AA7" s="37" t="str" cm="1">
+        <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="AB7" s="37" t="str" cm="1">
+        <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="AC7" s="49" t="str" cm="1">
+        <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="AD7" s="50" t="str" cm="1">
+        <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+      <c r="AE7" s="51" t="str" cm="1">
+        <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
+        <v>26 hours 20 minutes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="27">
         <v>45205</v>
@@ -1632,7 +1808,7 @@
         <v>0.69097222222222221</v>
       </c>
       <c r="E8" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.16111111111111109</v>
       </c>
       <c r="F8" s="15" t="str">
@@ -1646,34 +1822,74 @@
         <v>27</v>
       </c>
       <c r="I8"/>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="46" t="s">
+      <c r="K8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="47" t="s">
+      <c r="L8" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="53" t="s">
+      <c r="M8" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="47" t="s">
+      <c r="O8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="63" t="s">
+      <c r="P8" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="Q8" s="64" t="s">
+      <c r="Q8" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="48"/>
-    </row>
-    <row r="9" spans="1:18" s="41" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9"/>
+      <c r="R8" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="V8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="W8" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="X8" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y8" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z8" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA8" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB8" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC8" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD8" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE8" s="51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -1684,7 +1900,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="E9" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.18263888888888891</v>
       </c>
       <c r="F9" s="15" t="str">
@@ -1697,14 +1913,8 @@
       <c r="H9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I9"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="45"/>
-      <c r="P9" s="56"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="40"/>
-    </row>
-    <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -1715,7 +1925,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="E10" s="17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.6805555555555469E-2</v>
       </c>
       <c r="F10" s="15" t="str">
@@ -1729,7 +1939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -1754,46 +1964,84 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
       <c r="C12" s="16">
         <v>0.84375</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D12" s="12">
+        <v>0.89444444444444438</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="7"/>
+        <v>5.0694444444444375E-2</v>
       </c>
       <c r="F12" s="15" t="str">
         <f>IF(E12="","",_xlfn.CONCAT(HOUR(SUM($E$4:E12))," hours ",MINUTE(SUM($E$4:E12))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E13" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>22 hours 47 minutes</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="27">
+        <v>45208</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="7"/>
+        <v>1.736111111111116E-2</v>
       </c>
       <c r="F13" s="15" t="str">
         <f>IF(E13="","",_xlfn.CONCAT(HOUR(SUM($E$4:E13))," hours ",MINUTE(SUM($E$4:E13))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>23 hours 12 minutes</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="27">
+        <v>45208</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0.71666666666666667</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E14" s="17">
+        <f t="shared" si="7"/>
+        <v>0.13055555555555554</v>
       </c>
       <c r="F14" s="15" t="str">
         <f>IF(E14="","",_xlfn.CONCAT(HOUR(SUM($E$4:E14))," hours ",MINUTE(SUM($E$4:E14))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>2 hours 20 minutes</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E15" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F15" s="15" t="str">
@@ -1801,9 +2049,9 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="E16" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F16" s="15" t="str">
@@ -1813,7 +2061,7 @@
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F17" s="15" t="str">
@@ -1823,7 +2071,7 @@
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F18" s="15" t="str">
@@ -1833,7 +2081,7 @@
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F19" s="15" t="str">
@@ -1843,7 +2091,7 @@
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F20" s="15" t="str">
@@ -1853,7 +2101,7 @@
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F21" s="15" t="str">
@@ -1863,7 +2111,7 @@
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F22" s="15" t="str">
@@ -1873,7 +2121,7 @@
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F23" s="15" t="str">
@@ -1883,7 +2131,7 @@
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F24" s="15" t="str">
@@ -1893,7 +2141,7 @@
     </row>
     <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F25" s="15" t="str">
@@ -1903,7 +2151,7 @@
     </row>
     <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F26" s="15" t="str">
@@ -1913,7 +2161,7 @@
     </row>
     <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F27" s="15" t="str">
@@ -1923,7 +2171,7 @@
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F28" s="15" t="str">
@@ -1933,7 +2181,7 @@
     </row>
     <row r="29" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E29" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F29" s="15" t="str">
@@ -1943,7 +2191,7 @@
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E30" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F30" s="15" t="str">
@@ -1953,8 +2201,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H13" r:id="rId1" xr:uid="{40BF5D3F-6F40-4D36-A2D2-A18CA464B327}"/>
+  </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
a lot, check hour tracker
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b25eddf427344b8b/School Docs/Capstone/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="8_{6716760C-A5C1-4437-961B-D6AD7649868D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415F881F-E4C6-4021-A285-25A2EDAB793C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA614B85-D0ED-4F4A-99D3-1496FFAFDBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Start Time:</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Refactored the view panels to not be bad. Now the editor development can really start. I also sketched out what the pages might look like</t>
+  </si>
+  <si>
+    <t>It's weird to think this is a shared document. Not through excel, but github lol</t>
+  </si>
+  <si>
+    <t>Finished up the view panels, started on the sidebar, started laying out the editor page</t>
+  </si>
+  <si>
+    <t>Next items on the horizon are: file heirarchy viewer, theme switcher, settings, terminal, top bar, moving most state into a context, as well as starting on a lot of backend type shit</t>
   </si>
 </sst>
 </file>
@@ -927,10 +936,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1235,25 +1240,25 @@
   </sheetPr>
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
     <col min="6" max="6" width="20" style="15" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="53" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:31" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1267,7 +1272,7 @@
       <c r="H1" s="22"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2"/>
@@ -1288,7 +1293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="31" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1379,7 +1384,7 @@
         <v>45221</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -1442,7 +1447,7 @@
       </c>
       <c r="T4" s="35" t="str">
         <f t="shared" ref="T4:X4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, T$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>02 hours 15 minutes</v>
+        <v>04 hours 23 minutes</v>
       </c>
       <c r="U4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -1489,7 +1494,7 @@
         <v>00 hours 00 minutes</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -1601,7 +1606,7 @@
         <v>5 hours 0 minutes</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -1692,7 +1697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -1759,54 +1764,54 @@
       </c>
       <c r="T7" s="37" t="str" cm="1">
         <f t="array" ref="T7">INT((SUM(SUM(INT(LEFT($K$4:T$4, 2))), SUM(MID($K$4:T$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:T$4, 2))), SUM(MID($K$4:T$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="U7" s="37" t="str" cm="1">
         <f t="array" ref="U7">INT((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="V7" s="49" t="str" cm="1">
         <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
+        <v>36 hours 33 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>34 hours 25 minutes</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" s="39" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>36 hours 33 minutes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="27">
         <v>45205</v>
@@ -1899,7 +1904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -1924,7 +1929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -1949,7 +1954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
@@ -1999,7 +2004,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>45208</v>
       </c>
@@ -2024,7 +2029,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>45208</v>
       </c>
@@ -2049,7 +2054,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" ht="120" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>45209</v>
       </c>
@@ -2074,7 +2079,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -2096,7 +2101,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>45210</v>
       </c>
@@ -2117,18 +2122,36 @@
       <c r="G17" s="21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="17" t="str">
+      <c r="J17" s="53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B18" s="27">
+        <v>45210</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.77569444444444446</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="E18" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>8.8888888888888906E-2</v>
       </c>
       <c r="F18" s="15" t="str">
         <f>IF(E18="","",_xlfn.CONCAT(HOUR(SUM($E$4:E18))," hours ",MINUTE(SUM($E$4:E18))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+        <v>12 hours 33 minutes</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E19" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2138,7 +2161,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E20" s="17" t="str">
         <f>IF(OR(C20=0, D20=0),"", D20-C20)</f>
         <v/>
@@ -2148,7 +2171,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E21" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2158,7 +2181,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E22" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2168,7 +2191,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E23" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2178,7 +2201,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E24" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2188,7 +2211,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E25" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2198,7 +2221,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E26" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2208,7 +2231,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E27" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2218,7 +2241,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E28" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2228,7 +2251,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E29" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2238,7 +2261,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E30" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>

</xml_diff>

<commit_message>
Loading screen, and editor context
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA614B85-D0ED-4F4A-99D3-1496FFAFDBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8047A6AF-AF90-44E5-9AA5-3D31BFFA654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>Start Time:</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Next items on the horizon are: file heirarchy viewer, theme switcher, settings, terminal, top bar, moving most state into a context, as well as starting on a lot of backend type shit</t>
+  </si>
+  <si>
+    <t>Moved a lot of state to an editor context (I think all?), I also made a loading display for the react preview, and I moved the editor to /editor instead of /demo</t>
+  </si>
+  <si>
+    <t>Next is changing the react preview to mount a basic create-react-app file template instead of npm i. Along with that I should figure out how to use pnpm instead of npm</t>
   </si>
 </sst>
 </file>
@@ -1241,24 +1247,24 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="16" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="17" customWidth="1"/>
     <col min="6" max="6" width="20" style="15" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="37.81640625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.81640625" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" ht="36" x14ac:dyDescent="0.8">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1272,7 +1278,7 @@
       <c r="H1" s="22"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2"/>
@@ -1293,7 +1299,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1384,7 +1390,7 @@
         <v>45221</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -1451,7 +1457,7 @@
       </c>
       <c r="U4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 50 minutes</v>
       </c>
       <c r="V4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -1494,7 +1500,7 @@
         <v>00 hours 00 minutes</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="37" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -1563,7 +1569,7 @@
       </c>
       <c r="U5" s="37" t="str">
         <f t="shared" ref="U5:V5" si="5">IF(INT(LEFT(U$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>2 hours 0 minutes</v>
+        <v>0 hours 9.99999999999999 minutes</v>
       </c>
       <c r="V5" s="37" t="str">
         <f t="shared" si="5"/>
@@ -1606,7 +1612,7 @@
         <v>5 hours 0 minutes</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="37" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -1697,7 +1703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="39" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -1768,50 +1774,50 @@
       </c>
       <c r="U7" s="37" t="str" cm="1">
         <f t="array" ref="U7">INT((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="V7" s="49" t="str" cm="1">
         <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
+        <v>38 hours 23 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>36 hours 33 minutes</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+        <v>38 hours 23 minutes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" s="39" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A8"/>
       <c r="B8" s="27">
         <v>45205</v>
@@ -1904,7 +1910,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="58" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="58" x14ac:dyDescent="0.35">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="27">
         <v>45208</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="87" x14ac:dyDescent="0.35">
       <c r="B14" s="27">
         <v>45208</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B15" s="27">
         <v>45209</v>
       </c>
@@ -2079,7 +2085,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="87" x14ac:dyDescent="0.35">
       <c r="B17" s="27">
         <v>45210</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B18" s="27">
         <v>45210</v>
       </c>
@@ -2151,17 +2157,32 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="17" t="str">
+    <row r="19" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B19" s="27">
+        <v>45211</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E19" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>7.6388888888888784E-2</v>
       </c>
       <c r="F19" s="15" t="str">
         <f>IF(E19="","",_xlfn.CONCAT(HOUR(SUM($E$4:E19))," hours ",MINUTE(SUM($E$4:E19))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <v>14 hours 23 minutes</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E20" s="17" t="str">
         <f>IF(OR(C20=0, D20=0),"", D20-C20)</f>
         <v/>
@@ -2171,7 +2192,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E21" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2181,7 +2202,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E22" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2191,7 +2212,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E23" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2201,7 +2222,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E24" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2211,7 +2232,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E25" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2221,7 +2242,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E26" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2231,7 +2252,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E27" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2241,7 +2262,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E28" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2251,7 +2272,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E29" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2261,7 +2282,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E30" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>

</xml_diff>

<commit_message>
WebContainers mount a filesystem
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8047A6AF-AF90-44E5-9AA5-3D31BFFA654D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BBFE1E-E491-4708-99A9-240E4C511940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Start Time:</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>Next is changing the react preview to mount a basic create-react-app file template instead of npm i. Along with that I should figure out how to use pnpm instead of npm</t>
+  </si>
+  <si>
+    <t>I got the web containers mounting a react template that is stored as json instead of using npx create-react-app. I don't know if it's faster, but it is more controllable.</t>
+  </si>
+  <si>
+    <t>Next task is the file heirarchy viewer/selector. First view, then select opens it on the code editor</t>
   </si>
 </sst>
 </file>
@@ -1247,24 +1253,24 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
     <col min="6" max="6" width="20" style="15" customWidth="1"/>
-    <col min="7" max="7" width="37.81640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.81640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" style="53" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="36" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:31" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1278,7 +1284,7 @@
       <c r="H1" s="22"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2"/>
@@ -1299,7 +1305,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1390,7 +1396,7 @@
         <v>45221</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -1457,7 +1463,7 @@
       </c>
       <c r="U4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>01 hours 50 minutes</v>
+        <v>03 hours 35 minutes</v>
       </c>
       <c r="V4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -1500,7 +1506,7 @@
         <v>00 hours 00 minutes</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="37" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -1569,7 +1575,7 @@
       </c>
       <c r="U5" s="37" t="str">
         <f t="shared" ref="U5:V5" si="5">IF(INT(LEFT(U$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(U$6,1)-SUM(LEFT(U$4, 2), (MID(U4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>0 hours 9.99999999999999 minutes</v>
+        <v>Goal Met!</v>
       </c>
       <c r="V5" s="37" t="str">
         <f t="shared" si="5"/>
@@ -1612,7 +1618,7 @@
         <v>5 hours 0 minutes</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="37" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -1703,7 +1709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="39" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -1774,50 +1780,50 @@
       </c>
       <c r="U7" s="37" t="str" cm="1">
         <f t="array" ref="U7">INT((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:U$4, 2))), SUM(MID($K$4:U$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="V7" s="49" t="str" cm="1">
         <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
+        <v>40 hours 8 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>38 hours 23 minutes</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" s="39" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>40 hours 8 minutes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="27">
         <v>45205</v>
@@ -1910,7 +1916,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
@@ -2010,7 +2016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>45208</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>45208</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" ht="120" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>45209</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>45210</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="27">
         <v>45210</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>45211</v>
       </c>
@@ -2182,17 +2188,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E20" s="17" t="str">
+    <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B20" s="27">
+        <v>45211</v>
+      </c>
+      <c r="C20" s="16">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E20" s="17">
         <f>IF(OR(C20=0, D20=0),"", D20-C20)</f>
-        <v/>
+        <v>7.2916666666666741E-2</v>
       </c>
       <c r="F20" s="15" t="str">
         <f>IF(E20="","",_xlfn.CONCAT(HOUR(SUM($E$4:E20))," hours ",MINUTE(SUM($E$4:E20))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+        <v>16 hours 8 minutes</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E21" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2202,7 +2223,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E22" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2212,7 +2233,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E23" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2222,7 +2243,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E24" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2232,7 +2253,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E25" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2242,7 +2263,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E26" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2252,7 +2273,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E27" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2262,7 +2283,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E28" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2272,7 +2293,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E29" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -2282,7 +2303,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E30" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>

</xml_diff>

<commit_message>
Live editing of app,js works! also them tweaks
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BBFE1E-E491-4708-99A9-240E4C511940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1725381C-454D-4F6C-9039-009BEB39DEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <t>Start Time:</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>Next task is the file heirarchy viewer/selector. First view, then select opens it on the code editor</t>
+  </si>
+  <si>
+    <t>Got live editing working instead of doing what I said I needed to do next! Also did some theme tweaking</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1255,8 @@
   </sheetPr>
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +1470,7 @@
       </c>
       <c r="V4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 40 minutes</v>
       </c>
       <c r="W4" s="40" t="str">
         <f t="shared" si="1"/>
@@ -1579,7 +1582,7 @@
       </c>
       <c r="V5" s="37" t="str">
         <f t="shared" si="5"/>
-        <v>2 hours 0 minutes</v>
+        <v>Goal Met!</v>
       </c>
       <c r="W5" s="46" t="str">
         <f>IF(INT(LEFT(W$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
@@ -1784,43 +1787,43 @@
       </c>
       <c r="V7" s="49" t="str" cm="1">
         <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>40 hours 8 minutes</v>
+        <v>42 hours 48 minutes</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2213,14 +2216,26 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E21" s="17" t="str">
+    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="27">
+        <v>45212</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="E21" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F21" s="15" t="str">
         <f>IF(E21="","",_xlfn.CONCAT(HOUR(SUM($E$4:E21))," hours ",MINUTE(SUM($E$4:E21))," minutes"))</f>
-        <v/>
+        <v>18 hours 48 minutes</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
File Viewer in place
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1725381C-454D-4F6C-9039-009BEB39DEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168EF22-BEF8-47B0-9D2B-10E048E22738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>Start Time:</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>Got live editing working instead of doing what I said I needed to do next! Also did some theme tweaking</t>
+  </si>
+  <si>
+    <t>Got a lot of progress done on the file viewer/selector</t>
+  </si>
+  <si>
+    <t>Next is making it actually open a file, also the terminal</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1262,7 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1476,7 @@
       </c>
       <c r="V4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>02 hours 40 minutes</v>
+        <v>04 hours 35 minutes</v>
       </c>
       <c r="W4" s="40" t="str">
         <f t="shared" si="1"/>
@@ -1787,43 +1793,43 @@
       </c>
       <c r="V7" s="49" t="str" cm="1">
         <f t="array" ref="V7">INT((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:V$4, 2))), SUM(MID($K$4:V$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>42 hours 48 minutes</v>
+        <v>44 hours 43 minutes</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2238,14 +2244,29 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E22" s="17" t="str">
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="27">
+        <v>45212</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="E22" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>7.986111111111116E-2</v>
       </c>
       <c r="F22" s="15" t="str">
         <f>IF(E22="","",_xlfn.CONCAT(HOUR(SUM($E$4:E22))," hours ",MINUTE(SUM($E$4:E22))," minutes"))</f>
-        <v/>
+        <v>20 hours 43 minutes</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
file selection, code editor tabs, get all from fs
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168EF22-BEF8-47B0-9D2B-10E048E22738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69931AF9-738F-46A5-B063-780B48CC44FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
   <si>
     <t>Start Time:</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Next is making it actually open a file, also the terminal</t>
+  </si>
+  <si>
+    <t>Got the file explorer opening files! I also got it so files generated by npm i are shown to the user. Also you can select a specific file using tabs in the code editor</t>
+  </si>
+  <si>
+    <t>Next up is the terminal. Also I need to deal with technical debt soon if not now</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1267,8 @@
   </sheetPr>
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1486,7 @@
       </c>
       <c r="W4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>07 hours 00 minutes</v>
       </c>
       <c r="X4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -1592,7 +1598,7 @@
       </c>
       <c r="W5" s="46" t="str">
         <f>IF(INT(LEFT(W$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(W$6,1)-SUM(LEFT(W$4, 2), (MID(W4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>5 hours 0 minutes</v>
+        <v>Goal Met!</v>
       </c>
       <c r="X5" s="47" t="str">
         <f>IF(INT(LEFT(X$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(X$6,1)-SUM(LEFT(X$4, 2), (MID(X4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(X$6,1)-SUM(LEFT(X$4, 2), (MID(X4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
@@ -1797,39 +1803,39 @@
       </c>
       <c r="W7" s="50" t="str" cm="1">
         <f t="array" ref="W7">INT((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:W$4, 2))), SUM(MID($K$4:W$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="X7" s="51" t="str" cm="1">
         <f t="array" ref="X7">INT((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:X$4, 2))), SUM(MID($K$4:X$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>44 hours 43 minutes</v>
+        <v>51 hours 43 minutes</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2269,14 +2275,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E23" s="17" t="str">
+    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="27">
+        <v>45213</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0.53125</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E23" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.29166666666666663</v>
       </c>
       <c r="F23" s="15" t="str">
         <f>IF(E23="","",_xlfn.CONCAT(HOUR(SUM($E$4:E23))," hours ",MINUTE(SUM($E$4:E23))," minutes"))</f>
-        <v/>
+        <v>3 hours 43 minutes</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
preBig context changes post little context changes
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB66FFE-E781-437F-B6FD-4BD1A29620C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0B762-6183-44C6-A92C-943B1E59694D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
   <si>
     <t>Start Time:</t>
   </si>
@@ -204,9 +204,6 @@
     <t>42 hours</t>
   </si>
   <si>
-    <t>44 hours</t>
-  </si>
-  <si>
     <t>46 hours</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>Week 3</t>
   </si>
   <si>
-    <t>55 hours</t>
-  </si>
-  <si>
     <t>60 hours</t>
   </si>
   <si>
@@ -283,6 +277,15 @@
   </si>
   <si>
     <t>Auto fileviewer refresh is on the horizon, but not something I want to immediately tackle. Next will be fixing technical debt</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>53 hours</t>
+  </si>
+  <si>
+    <t>58 hours</t>
   </si>
 </sst>
 </file>
@@ -1273,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,13 +1320,13 @@
       <c r="H2" s="22"/>
       <c r="J2" s="29"/>
       <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
         <v>52</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Y2" t="s">
         <v>53</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:31" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1616,7 +1619,7 @@
       </c>
       <c r="Z5" s="37" t="str">
         <f>IF(INT(LEFT(Z$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>2 hours 0 minutes</v>
+        <v>4 hours 0 minutes</v>
       </c>
       <c r="AA5" s="43" t="str">
         <f>IF(INT(LEFT(AA$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(AA$6,1)-SUM(LEFT(AA$4, 2), (MID(AA4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AA$6,1)-SUM(LEFT(AA$4, 2), (MID(AA4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
@@ -1628,7 +1631,7 @@
       </c>
       <c r="AC5" s="37" t="str">
         <f t="shared" si="6"/>
-        <v>2 hours 0 minutes</v>
+        <v>3 hours 0 minutes</v>
       </c>
       <c r="AD5" s="46" t="str">
         <f>IF(INT(LEFT(AD$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(AD$6,1)-SUM(LEFT(AD$4, 2), (MID(AD4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AD$6,1)-SUM(LEFT(AD$4, 2), (MID(AD4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
@@ -1636,7 +1639,7 @@
       </c>
       <c r="AE5" s="47" t="str">
         <f>IF(INT(LEFT(AE$4, 2)) &gt;= 5, "Goal Met!", ROUND((LEFT(AE$6,1)-SUM(LEFT(AE$4, 2), (MID(AE4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AE$6,1)-SUM(LEFT(AE$4, 2), (MID(AE4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>5 hours 0 minutes</v>
+        <v>2 hours 0 minutes</v>
       </c>
     </row>
     <row r="6" spans="1:31" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -1712,7 +1715,7 @@
         <v>17</v>
       </c>
       <c r="Z6" s="37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AA6" s="37" t="s">
         <v>17</v>
@@ -1721,13 +1724,13 @@
         <v>17</v>
       </c>
       <c r="AC6" s="37" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="AD6" s="46" t="s">
         <v>19</v>
       </c>
       <c r="AE6" s="47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:31" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1928,13 +1931,13 @@
         <v>50</v>
       </c>
       <c r="AC8" s="39" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="AD8" s="50" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="AE8" s="51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
@@ -2106,10 +2109,10 @@
         <v>5 hours 35 minutes</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="30" x14ac:dyDescent="0.25">
@@ -2131,7 +2134,7 @@
         <v>8 hours 10 minutes</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="90" x14ac:dyDescent="0.25">
@@ -2153,10 +2156,10 @@
         <v>10 hours 25 minutes</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J17" s="53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2178,10 +2181,10 @@
         <v>12 hours 33 minutes</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2203,10 +2206,10 @@
         <v>14 hours 23 minutes</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2228,10 +2231,10 @@
         <v>16 hours 8 minutes</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -2253,7 +2256,7 @@
         <v>18 hours 48 minutes</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -2275,10 +2278,10 @@
         <v>20 hours 43 minutes</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2300,10 +2303,10 @@
         <v>3 hours 43 minutes</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2325,13 +2328,19 @@
         <v>7 hours 8 minutes</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="27">
+        <v>45215</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0.80555555555555547</v>
+      </c>
       <c r="E25" s="17" t="str">
         <f t="shared" si="7"/>
         <v/>

</xml_diff>

<commit_message>
Refactored state and webcontainer/terminal
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB0B762-6183-44C6-A92C-943B1E59694D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6C57D2-E8C2-409B-BB74-4E3CA1FE0A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>Start Time:</t>
   </si>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>58 hours</t>
+  </si>
+  <si>
+    <t>I think the next thing on the quest to refactor is addressing all clouds/thought bubbles 💭</t>
+  </si>
+  <si>
+    <t>Refactored the state of the application to be less of a massive headache. Implemented custom hooks to grab select groups of values from the context. I also moved fragile code to a context.</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1282,8 @@
   </sheetPr>
   <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1509,7 @@
       </c>
       <c r="Y4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Y$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 50 minutes</v>
       </c>
       <c r="Z4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Z$3), "hh ""hours ""mm ""minutes""")</f>
@@ -1615,7 +1621,7 @@
       </c>
       <c r="Y5" s="45" t="str">
         <f>IF(INT(LEFT(Y$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(Y$6,1)-SUM(LEFT(Y$4, 2), (MID(Y4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Y$6,1)-SUM(LEFT(Y$4, 2), (MID(Y4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>2 hours 0 minutes</v>
+        <v>Goal Met!</v>
       </c>
       <c r="Z5" s="37" t="str">
         <f>IF(INT(LEFT(Z$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(Z$6,1)-SUM(LEFT(Z$4, 2), (MID(Z4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
@@ -1820,31 +1826,31 @@
       </c>
       <c r="Y7" s="48" t="str" cm="1">
         <f t="array" ref="Y7">INT((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Y$4, 2))), SUM(MID($K$4:Y$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="Z7" s="37" t="str" cm="1">
         <f t="array" ref="Z7">INT((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:Z$4, 2))), SUM(MID($K$4:Z$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="AA7" s="37" t="str" cm="1">
         <f t="array" ref="AA7">INT((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AA$4, 2))), SUM(MID($K$4:AA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>55 hours 8 minutes</v>
+        <v>58 hours 58 minutes</v>
       </c>
     </row>
     <row r="8" spans="1:31" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2334,20 +2340,29 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
       <c r="C25" s="16">
         <v>0.80555555555555547</v>
       </c>
-      <c r="E25" s="17" t="str">
+      <c r="D25" s="12">
+        <v>0.96527777777777779</v>
+      </c>
+      <c r="E25" s="17">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0.15972222222222232</v>
       </c>
       <c r="F25" s="15" t="str">
         <f>IF(E25="","",_xlfn.CONCAT(HOUR(SUM($E$4:E25))," hours ",MINUTE(SUM($E$4:E25))," minutes"))</f>
-        <v/>
+        <v>10 hours 58 minutes</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
got backend auth started
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337E616D-16BC-4D8A-992C-D2FA2659AE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAE0C6E-C2F2-4F0F-9AE1-265A1A64D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="97">
   <si>
     <t>Start Time:</t>
   </si>
@@ -339,10 +339,16 @@
     <t>https://next-auth.js.org/configuration/providers/oauth</t>
   </si>
   <si>
-    <t>Got Oauth started</t>
-  </si>
-  <si>
     <t>Next session it's time to make the database side of accounts, this include credential sign ins and connecting Oauth accounts</t>
+  </si>
+  <si>
+    <t>Got backend auth started</t>
+  </si>
+  <si>
+    <t>Got Oauth working on the frontend</t>
+  </si>
+  <si>
+    <t>Next is finishing backend auth</t>
   </si>
 </sst>
 </file>
@@ -1336,25 +1342,25 @@
   </sheetPr>
   <dimension ref="A1:EU30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="16" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="17" customWidth="1"/>
     <col min="6" max="6" width="20" style="15" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.88671875" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:151" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:151" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1368,7 +1374,7 @@
       <c r="H1" s="22"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:151" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2"/>
@@ -1389,7 +1395,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:151" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:151" s="31" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -1642,7 +1648,7 @@
       <c r="ES3" s="41"/>
       <c r="ET3" s="41"/>
     </row>
-    <row r="4" spans="1:151" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:151" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -1737,7 +1743,7 @@
       </c>
       <c r="AB4" s="35" t="str">
         <f t="shared" si="2"/>
-        <v>00 hours 00 minutes</v>
+        <v>00 hours 51 minutes</v>
       </c>
       <c r="AC4" s="35" t="str">
         <f t="shared" si="2"/>
@@ -1961,7 +1967,7 @@
       <c r="ES4" s="40"/>
       <c r="ET4" s="42"/>
     </row>
-    <row r="5" spans="1:151" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:151" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -2058,7 +2064,7 @@
       </c>
       <c r="AB5" s="37" t="str">
         <f t="shared" ref="AB5:AC5" si="7">IF(INT(LEFT(AB$4, 2)) &gt;= 2, "Goal Met!", ROUND((LEFT(AB$6,1)-SUM(LEFT(AB$4, 2), (MID(AB4,10,2)/60))), 0) &amp; " hours " &amp; MOD((LEFT(AB$6,1)-SUM(LEFT(AB$4, 2), (MID(AB4,10,2)/60))) * 60, 60) &amp; " minutes")</f>
-        <v>2 hours 0 minutes</v>
+        <v>1 hours 9 minutes</v>
       </c>
       <c r="AC5" s="37" t="str">
         <f t="shared" si="7"/>
@@ -2304,7 +2310,7 @@
       <c r="ET5" s="47"/>
       <c r="EU5" s="45"/>
     </row>
-    <row r="6" spans="1:151" s="37" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:151" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -2569,7 +2575,7 @@
       <c r="ET6" s="47"/>
       <c r="EU6" s="36"/>
     </row>
-    <row r="7" spans="1:151" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:151" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -2670,207 +2676,207 @@
       </c>
       <c r="AB7" s="37" t="str" cm="1">
         <f t="array" ref="AB7">INT((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AB$4, 2))), SUM(MID($K$4:AB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AC7" s="49" t="str" cm="1">
         <f t="array" ref="AC7">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AD7" s="50" t="str" cm="1">
         <f t="array" ref="AD7">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AE7" s="51" t="str" cm="1">
         <f t="array" ref="AE7">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AF7" s="48" t="str" cm="1">
         <f t="array" ref="AF7">INT((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AG7" s="37" t="str" cm="1">
         <f t="array" ref="AG7">INT((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AH7" s="37" t="str" cm="1">
         <f t="array" ref="AH7">INT((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AI7" s="37" t="str" cm="1">
         <f t="array" ref="AI7">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AJ7" s="49" t="str" cm="1">
         <f t="array" ref="AJ7">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AK7" s="50" t="str" cm="1">
         <f t="array" ref="AK7">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AL7" s="51" t="str" cm="1">
         <f t="array" ref="AL7">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AM7" s="48" t="str" cm="1">
         <f t="array" ref="AM7">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AN7" s="37" t="str" cm="1">
         <f t="array" ref="AN7">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AO7" s="37" t="str" cm="1">
         <f t="array" ref="AO7">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AP7" s="37" t="str" cm="1">
         <f t="array" ref="AP7">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AQ7" s="49" t="str" cm="1">
         <f t="array" ref="AQ7">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AR7" s="50" t="str" cm="1">
         <f t="array" ref="AR7">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AS7" s="51" t="str" cm="1">
         <f t="array" ref="AS7">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AT7" s="48" t="str" cm="1">
         <f t="array" ref="AT7">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AU7" s="37" t="str" cm="1">
         <f t="array" ref="AU7">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AV7" s="37" t="str" cm="1">
         <f t="array" ref="AV7">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AW7" s="37" t="str" cm="1">
         <f t="array" ref="AW7">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AX7" s="49" t="str" cm="1">
         <f t="array" ref="AX7">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AY7" s="50" t="str" cm="1">
         <f t="array" ref="AY7">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="AZ7" s="51" t="str" cm="1">
         <f t="array" ref="AZ7">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BA7" s="48" t="str" cm="1">
         <f t="array" ref="BA7">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BB7" s="37" t="str" cm="1">
         <f t="array" ref="BB7">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BC7" s="37" t="str" cm="1">
         <f t="array" ref="BC7">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BD7" s="37" t="str" cm="1">
         <f t="array" ref="BD7">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BE7" s="49" t="str" cm="1">
         <f t="array" ref="BE7">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BF7" s="50" t="str" cm="1">
         <f t="array" ref="BF7">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BG7" s="51" t="str" cm="1">
         <f t="array" ref="BG7">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BH7" s="48" t="str" cm="1">
         <f t="array" ref="BH7">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BI7" s="37" t="str" cm="1">
         <f t="array" ref="BI7">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BJ7" s="37" t="str" cm="1">
         <f t="array" ref="BJ7">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BK7" s="37" t="str" cm="1">
         <f t="array" ref="BK7">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BL7" s="49" t="str" cm="1">
         <f t="array" ref="BL7">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BM7" s="50" t="str" cm="1">
         <f t="array" ref="BM7">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BN7" s="51" t="str" cm="1">
         <f t="array" ref="BN7">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BO7" s="48" t="str" cm="1">
         <f t="array" ref="BO7">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BP7" s="37" t="str" cm="1">
         <f t="array" ref="BP7">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BQ7" s="37" t="str" cm="1">
         <f t="array" ref="BQ7">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BR7" s="37" t="str" cm="1">
         <f t="array" ref="BR7">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BS7" s="49" t="str" cm="1">
         <f t="array" ref="BS7">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BT7" s="50" t="str" cm="1">
         <f t="array" ref="BT7">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BU7" s="51" t="str" cm="1">
         <f t="array" ref="BU7">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BV7" s="48" t="str" cm="1">
         <f t="array" ref="BV7">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BW7" s="37" t="str" cm="1">
         <f t="array" ref="BW7">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BX7" s="37" t="str" cm="1">
         <f t="array" ref="BX7">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BY7" s="37" t="str" cm="1">
         <f t="array" ref="BY7">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="BZ7" s="49" t="str" cm="1">
         <f t="array" ref="BZ7">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>65 hours 48 minutes</v>
+        <v>66 hours 39.0000000000005 minutes</v>
       </c>
       <c r="CA7" s="50"/>
       <c r="CB7" s="51"/>
@@ -2946,7 +2952,7 @@
       <c r="ET7" s="51"/>
       <c r="EU7" s="48"/>
     </row>
-    <row r="8" spans="1:151" s="39" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:151" s="39" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8"/>
       <c r="B8" s="27">
         <v>45205</v>
@@ -3062,7 +3068,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:151" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:151" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:151" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:151" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -3118,7 +3124,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:151" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:151" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -3146,7 +3152,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:151" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:151" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
@@ -3174,7 +3180,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:151" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:151" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
         <v>45208</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:151" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:151" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
         <v>45208</v>
       </c>
@@ -3230,7 +3236,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:151" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:151" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B15" s="27">
         <v>45209</v>
       </c>
@@ -3258,7 +3264,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:151" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:151" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B17" s="27">
         <v>45210</v>
       </c>
@@ -3305,7 +3311,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B18" s="27">
         <v>45210</v>
       </c>
@@ -3333,7 +3339,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B19" s="27">
         <v>45211</v>
       </c>
@@ -3361,7 +3367,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="27">
         <v>45211</v>
       </c>
@@ -3389,7 +3395,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="27">
         <v>45212</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="27">
         <v>45212</v>
       </c>
@@ -3439,7 +3445,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B23" s="27">
         <v>45213</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B24" s="27">
         <v>45214</v>
       </c>
@@ -3495,7 +3501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="27">
         <v>45216</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B27" s="27">
         <v>45216</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B28" s="27">
         <v>45217</v>
       </c>
@@ -3589,26 +3595,41 @@
         <v>17 hours 48 minutes</v>
       </c>
       <c r="G28" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="25" t="s">
         <v>93</v>
-      </c>
-      <c r="H28" s="25" t="s">
-        <v>94</v>
       </c>
       <c r="J28" s="55" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E29" s="17" t="str">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="27">
+        <v>45218</v>
+      </c>
+      <c r="C29" s="16">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0.45902777777777781</v>
+      </c>
+      <c r="E29" s="17">
         <f t="shared" si="20"/>
-        <v/>
+        <v>3.5416666666666707E-2</v>
       </c>
       <c r="F29" s="15" t="str">
         <f>IF(E29="","",_xlfn.CONCAT(HOUR(SUM($E$4:E29))," hours ",MINUTE(SUM($E$4:E29))," minutes"))</f>
-        <v/>
+        <v>18 hours 39 minutes</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E30" s="17" t="str">
         <f t="shared" si="20"/>
         <v/>

</xml_diff>

<commit_message>
backend auth talks to frontend or vice versa
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1927D429-1221-492F-9B7B-31424F91960A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FF441-FC4A-42BD-BD51-2D925FBCC385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
   <si>
     <t>Start Time:</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Keep going with backend Account system</t>
+  </si>
+  <si>
+    <t>Got authentication and session figured out between the backend and the frontend</t>
+  </si>
+  <si>
+    <t>Next step is getting OAuth accounts created in our backend, and merging accounts with the same email</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1342,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1747,7 @@
       </c>
       <c r="AC4" s="35" t="str">
         <f t="shared" si="2"/>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 30 minutes</v>
       </c>
       <c r="AD4" s="40" t="str">
         <f t="shared" si="2"/>
@@ -2327,203 +2333,203 @@
       </c>
       <c r="AC6" s="47" t="str" cm="1">
         <f t="array" ref="AC6">INT((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AC$4, 2))), SUM(MID($K$4:AC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AD6" s="48" t="str" cm="1">
         <f t="array" ref="AD6">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AE6" s="49" t="str" cm="1">
         <f t="array" ref="AE6">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AF6" s="46" t="str" cm="1">
         <f t="array" ref="AF6">INT((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AG6" s="37" t="str" cm="1">
         <f t="array" ref="AG6">INT((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AH6" s="37" t="str" cm="1">
         <f t="array" ref="AH6">INT((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AI6" s="37" t="str" cm="1">
         <f t="array" ref="AI6">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AJ6" s="47" t="str" cm="1">
         <f t="array" ref="AJ6">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>68 hours 9.00000000000045 minutes</v>
+        <v>71 hours 39 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3176,7 +3182,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
@@ -3354,14 +3360,29 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E32" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="32" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="27">
+        <v>45219</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="E32" s="17">
+        <f t="shared" si="5"/>
+        <v>0.14583333333333331</v>
       </c>
       <c r="F32" s="15" t="str">
         <f>IF(E32="","",_xlfn.CONCAT(HOUR(SUM($E$4:E32))," hours ",MINUTE(SUM($E$4:E32))," minutes"))</f>
-        <v/>
+        <v>23 hours 39 minutes</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="5:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lots of account/project progress
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174FF441-FC4A-42BD-BD51-2D925FBCC385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52951921-1DF5-47DD-8684-27363C5F76B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="116">
   <si>
     <t>Start Time:</t>
   </si>
@@ -364,6 +364,48 @@
   </si>
   <si>
     <t>Next step is getting OAuth accounts created in our backend, and merging accounts with the same email</t>
+  </si>
+  <si>
+    <t>Only taking a break to bathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Got a lot of project API made, added some to auth/account API</t>
+  </si>
+  <si>
+    <t>Next is adding projects to users, then getting the frontend "register -&gt; login -&gt; create project -&gt; open project" flow</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>I think the project should go gold this week</t>
+  </si>
+  <si>
+    <t>Got the register frontend wired to backend alongsied making the security code for the non auth apis, a new project endpoint, and some more account and project endpoints</t>
+  </si>
+  <si>
+    <t>Next is the dashboard/account page</t>
   </si>
 </sst>
 </file>
@@ -1342,8 +1384,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,6 +1435,30 @@
       </c>
       <c r="Y2" t="s">
         <v>52</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>113</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>110</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:151" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1751,7 +1817,7 @@
       </c>
       <c r="AD4" s="40" t="str">
         <f t="shared" si="2"/>
-        <v>00 hours 00 minutes</v>
+        <v>05 hours 07 minutes</v>
       </c>
       <c r="AE4" s="42" t="str">
         <f t="shared" si="2"/>
@@ -2337,199 +2403,199 @@
       </c>
       <c r="AD6" s="48" t="str" cm="1">
         <f t="array" ref="AD6">INT((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AD$4, 2))), SUM(MID($K$4:AD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AE6" s="49" t="str" cm="1">
         <f t="array" ref="AE6">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AF6" s="46" t="str" cm="1">
         <f t="array" ref="AF6">INT((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AG6" s="37" t="str" cm="1">
         <f t="array" ref="AG6">INT((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AH6" s="37" t="str" cm="1">
         <f t="array" ref="AH6">INT((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AI6" s="37" t="str" cm="1">
         <f t="array" ref="AI6">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AJ6" s="47" t="str" cm="1">
         <f t="array" ref="AJ6">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>71 hours 39 minutes</v>
+        <v>76 hours 46 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2945,7 +3011,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:151" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:151" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -3126,7 +3192,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>45213</v>
       </c>
@@ -3154,7 +3220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>45214</v>
       </c>
@@ -3385,37 +3451,82 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="27">
+        <v>45220</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="E33" s="17">
+        <f t="shared" si="5"/>
+        <v>2.2222222222222254E-2</v>
       </c>
       <c r="F33" s="15" t="str">
         <f>IF(E33="","",_xlfn.CONCAT(HOUR(SUM($E$4:E33))," hours ",MINUTE(SUM($E$4:E33))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>0 hours 11 minutes</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="27">
+        <v>45220</v>
+      </c>
+      <c r="C34" s="16">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D34" s="12">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="E34" s="17">
+        <f t="shared" si="5"/>
+        <v>0.10763888888888884</v>
       </c>
       <c r="F34" s="15" t="str">
         <f>IF(E34="","",_xlfn.CONCAT(HOUR(SUM($E$4:E34))," hours ",MINUTE(SUM($E$4:E34))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E35" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>2 hours 46 minutes</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B35" s="27">
+        <v>45220</v>
+      </c>
+      <c r="C35" s="16">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="E35" s="17">
+        <f t="shared" si="5"/>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="F35" s="15" t="str">
         <f>IF(E35="","",_xlfn.CONCAT(HOUR(SUM($E$4:E35))," hours ",MINUTE(SUM($E$4:E35))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+        <v>4 hours 46 minutes</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E36" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3425,7 +3536,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E37" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3435,7 +3546,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E38" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3445,7 +3556,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E39" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3455,7 +3566,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E40" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3465,7 +3576,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E41" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3475,7 +3586,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E42" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3485,7 +3596,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E43" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3495,7 +3606,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E44" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3505,7 +3616,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E45" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3515,7 +3626,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E46" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3525,7 +3636,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E47" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3535,7 +3646,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>

</xml_diff>

<commit_message>
Editor loads project, dashboard lists them
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52951921-1DF5-47DD-8684-27363C5F76B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9123B-AD7D-4209-8A90-0EA1A6DEB64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="120">
   <si>
     <t>Start Time:</t>
   </si>
@@ -406,6 +406,18 @@
   </si>
   <si>
     <t>Next is the dashboard/account page</t>
+  </si>
+  <si>
+    <t>Got started on dashboard, mostly only got design ideas started. I got stuck then the internet died</t>
+  </si>
+  <si>
+    <t>Make the dashboard page</t>
+  </si>
+  <si>
+    <t>The dashboard shows the logged in users projects. The editor page can now load from a user's saved project</t>
+  </si>
+  <si>
+    <t>Next is the "new project" button, as well as figuring out how to make the attrocious loading times a better experience</t>
   </si>
 </sst>
 </file>
@@ -1384,8 +1396,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,7 +1833,7 @@
       </c>
       <c r="AE4" s="42" t="str">
         <f t="shared" si="2"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 25 minutes</v>
       </c>
       <c r="AF4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AF$3), "hh ""hours ""mm ""minutes""")</f>
@@ -2407,195 +2419,195 @@
       </c>
       <c r="AE6" s="49" t="str" cm="1">
         <f t="array" ref="AE6">INT((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AE$4, 2))), SUM(MID($K$4:AE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AF6" s="46" t="str" cm="1">
         <f t="array" ref="AF6">INT((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AF$4, 2))), SUM(MID($K$4:AF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AG6" s="37" t="str" cm="1">
         <f t="array" ref="AG6">INT((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AH6" s="37" t="str" cm="1">
         <f t="array" ref="AH6">INT((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AI6" s="37" t="str" cm="1">
         <f t="array" ref="AI6">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AJ6" s="47" t="str" cm="1">
         <f t="array" ref="AJ6">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>76 hours 46 minutes</v>
+        <v>79 hours 11 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3526,24 +3538,54 @@
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E36" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="27">
+        <v>45221</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D36" s="12">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E36" s="17">
+        <f t="shared" si="5"/>
+        <v>3.4722222222222154E-2</v>
       </c>
       <c r="F36" s="15" t="str">
         <f>IF(E36="","",_xlfn.CONCAT(HOUR(SUM($E$4:E36))," hours ",MINUTE(SUM($E$4:E36))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>5 hours 36 minutes</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B37" s="27">
+        <v>45221</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D37" s="12">
+        <v>0.89236111111111116</v>
+      </c>
+      <c r="E37" s="17">
+        <f t="shared" si="5"/>
+        <v>6.5972222222222321E-2</v>
       </c>
       <c r="F37" s="15" t="str">
         <f>IF(E37="","",_xlfn.CONCAT(HOUR(SUM($E$4:E37))," hours ",MINUTE(SUM($E$4:E37))," minutes"))</f>
-        <v/>
+        <v>7 hours 11 minutes</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added templates, isAdmin, collaborators to backend
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D31E5B-3965-4B12-B6DE-073C1E855ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC75311-F469-4794-851D-CDF14B50FB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
   <si>
     <t>Start Time:</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>I want to add a template system, coming up soon will also be adding files and folders in the editor, as well as finally getting to the navbar</t>
+  </si>
+  <si>
+    <t>Implemented most if not all of the template backend</t>
+  </si>
+  <si>
+    <t>Next is template frontend stuff, I think I will start with the new template stuff to finish off the new project form, then jump to finishing up the editor. This is a nice transition since the editor needs a "Set as template" space</t>
   </si>
 </sst>
 </file>
@@ -1402,8 +1408,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,11 +1853,11 @@
       </c>
       <c r="AG4" s="35" t="str">
         <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AG$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>04 hours 20 minutes</v>
+        <v>04 hours 17 minutes</v>
       </c>
       <c r="AH4" s="35" t="str">
         <f t="shared" ref="AH4:BZ4" si="3">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AH$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 08 minutes</v>
       </c>
       <c r="AI4" s="35" t="str">
         <f t="shared" si="3"/>
@@ -2433,187 +2439,187 @@
       </c>
       <c r="AG6" s="37" t="str" cm="1">
         <f t="array" ref="AG6">INT((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AG$4, 2))), SUM(MID($K$4:AG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>83 hours 28 minutes</v>
       </c>
       <c r="AH6" s="37" t="str" cm="1">
         <f t="array" ref="AH6">INT((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AH$4, 2))), SUM(MID($K$4:AH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AI6" s="37" t="str" cm="1">
         <f t="array" ref="AI6">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AJ6" s="47" t="str" cm="1">
         <f t="array" ref="AJ6">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>83 hours 31 minutes</v>
+        <v>85 hours 36 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3602,15 +3608,15 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="D38" s="12">
-        <v>0.85069444444444453</v>
+        <v>0.84861111111111109</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="5"/>
-        <v>0.18055555555555569</v>
+        <v>0.17847222222222225</v>
       </c>
       <c r="F38" s="15" t="str">
         <f>IF(E38="","",_xlfn.CONCAT(HOUR(SUM($E$4:E38))," hours ",MINUTE(SUM($E$4:E38))," minutes"))</f>
-        <v>11 hours 31 minutes</v>
+        <v>11 hours 28 minutes</v>
       </c>
       <c r="G38" s="21" t="s">
         <v>120</v>
@@ -3619,14 +3625,29 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="39" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="B39" s="27">
+        <v>45224</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D39" s="12">
+        <v>0.81805555555555554</v>
+      </c>
+      <c r="E39" s="17">
+        <f t="shared" si="5"/>
+        <v>8.8888888888888906E-2</v>
       </c>
       <c r="F39" s="15" t="str">
         <f>IF(E39="","",_xlfn.CONCAT(HOUR(SUM($E$4:E39))," hours ",MINUTE(SUM($E$4:E39))," minutes"))</f>
-        <v/>
+        <v>13 hours 36 minutes</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="H39" s="25" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
So much, check the hour tracker
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC75311-F469-4794-851D-CDF14B50FB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0397D0FD-7119-40BF-B440-CE3E62B0FAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="127">
   <si>
     <t>Start Time:</t>
   </si>
@@ -430,6 +430,15 @@
   </si>
   <si>
     <t>Next is template frontend stuff, I think I will start with the new template stuff to finish off the new project form, then jump to finishing up the editor. This is a nice transition since the editor needs a "Set as template" space</t>
+  </si>
+  <si>
+    <t>Started work on ProjectList, then got distracted trying to adjust for timezone. I failed. I also made some backend tweaks to data types, might do more</t>
+  </si>
+  <si>
+    <t>I fixed the timestamps, some datatypes, made a shared models folder so I can have the same models between my python APIs, and modified the loading component</t>
+  </si>
+  <si>
+    <t>Next I want to finish the auto sign out, after that I think I wanna do the editor navbar and other editor things</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1418,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,11 +1870,11 @@
       </c>
       <c r="AI4" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 25 minutes</v>
       </c>
       <c r="AJ4" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
+        <v>04 hours 20 minutes</v>
       </c>
       <c r="AK4" s="40" t="str">
         <f t="shared" si="3"/>
@@ -2447,179 +2456,179 @@
       </c>
       <c r="AI6" s="37" t="str" cm="1">
         <f t="array" ref="AI6">INT((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AI$4, 2))), SUM(MID($K$4:AI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>88 hours 1 minutes</v>
       </c>
       <c r="AJ6" s="47" t="str" cm="1">
         <f t="array" ref="AJ6">INT((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AJ$4, 2))), SUM(MID($K$4:AJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>85 hours 36 minutes</v>
+        <v>92 hours 21 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3650,24 +3659,51 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B40" s="27">
+        <v>45225</v>
+      </c>
+      <c r="C40" s="16">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D40" s="12">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E40" s="17">
+        <f t="shared" si="5"/>
+        <v>0.10069444444444442</v>
       </c>
       <c r="F40" s="15" t="str">
         <f>IF(E40="","",_xlfn.CONCAT(HOUR(SUM($E$4:E40))," hours ",MINUTE(SUM($E$4:E40))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>16 hours 1 minutes</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B41" s="27">
+        <v>45226</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D41" s="12">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E41" s="17">
+        <f t="shared" si="5"/>
+        <v>0.18055555555555558</v>
       </c>
       <c r="F41" s="15" t="str">
         <f>IF(E41="","",_xlfn.CONCAT(HOUR(SUM($E$4:E41))," hours ",MINUTE(SUM($E$4:E41))," minutes"))</f>
-        <v/>
+        <v>20 hours 21 minutes</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed autosignout, and changed redirect + more
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0397D0FD-7119-40BF-B440-CE3E62B0FAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A7B393-C40F-43E8-A945-9B75C523A729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="144">
   <si>
     <t>Start Time:</t>
   </si>
@@ -318,9 +318,6 @@
     <t>73 hours</t>
   </si>
   <si>
-    <t>78 hours</t>
-  </si>
-  <si>
     <t>80 hours</t>
   </si>
   <si>
@@ -439,6 +436,60 @@
   </si>
   <si>
     <t>Next I want to finish the auto sign out, after that I think I wanna do the editor navbar and other editor things</t>
+  </si>
+  <si>
+    <t>77 hours</t>
+  </si>
+  <si>
+    <t>82 hours</t>
+  </si>
+  <si>
+    <t>86 hours</t>
+  </si>
+  <si>
+    <t>88 hours</t>
+  </si>
+  <si>
+    <t>90 hours</t>
+  </si>
+  <si>
+    <t>93 hours</t>
+  </si>
+  <si>
+    <t>98 hours</t>
+  </si>
+  <si>
+    <t>100 hours</t>
+  </si>
+  <si>
+    <t>102 hours</t>
+  </si>
+  <si>
+    <t>106 hours</t>
+  </si>
+  <si>
+    <t>108 hours</t>
+  </si>
+  <si>
+    <t>110 hours</t>
+  </si>
+  <si>
+    <t>113 hours</t>
+  </si>
+  <si>
+    <t>118 hours</t>
+  </si>
+  <si>
+    <t>120 hours</t>
+  </si>
+  <si>
+    <t>Next is navbar functionality, the profile component, more dashboard progress, making the settings sidebar panel, and redoing the terminal scrollbar</t>
+  </si>
+  <si>
+    <t>Not actually all of these, I'm just listing some options</t>
+  </si>
+  <si>
+    <t>Started the topbar frontend bits, created a new context hook for project metadata, changed how redirects work, also fixed auto sign out I think</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1468,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,28 +1521,28 @@
         <v>52</v>
       </c>
       <c r="AF2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM2" t="s">
         <v>106</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AT2" t="s">
         <v>107</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BA2" t="s">
         <v>108</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
+        <v>112</v>
+      </c>
+      <c r="BH2" t="s">
         <v>109</v>
       </c>
-      <c r="BB2" t="s">
-        <v>113</v>
-      </c>
-      <c r="BH2" t="s">
+      <c r="BO2" t="s">
         <v>110</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BV2" t="s">
         <v>111</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:151" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1878,7 +1929,7 @@
       </c>
       <c r="AK4" s="40" t="str">
         <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 15 minutes</v>
       </c>
       <c r="AL4" s="42" t="str">
         <f t="shared" si="3"/>
@@ -2172,10 +2223,10 @@
         <v>72</v>
       </c>
       <c r="AK5" s="44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AL5" s="45" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="AM5" s="36" t="s">
         <v>16</v>
@@ -2464,171 +2515,171 @@
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>92 hours 21 minutes</v>
+        <v>95 hours 36 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2814,10 +2865,52 @@
         <v>85</v>
       </c>
       <c r="AK7" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL7" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="AL7" s="39" t="s">
-        <v>87</v>
+      <c r="AM7" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="AN7" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="AO7" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP7" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ7" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR7" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="AS7" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="AT7" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU7" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="AV7" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="AW7" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX7" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="AY7" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="AZ7" s="39" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
@@ -3116,7 +3209,7 @@
         <v>60</v>
       </c>
       <c r="I18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3278,7 +3371,7 @@
         <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3306,7 +3399,7 @@
         <v>75</v>
       </c>
       <c r="I25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -3356,7 +3449,7 @@
         <v>80</v>
       </c>
       <c r="J27" s="53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3378,10 +3471,10 @@
         <v>17 hours 48 minutes</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -3403,10 +3496,10 @@
         <v>18 hours 39 minutes</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3428,10 +3521,10 @@
         <v>19 hours 9 minutes</v>
       </c>
       <c r="G30" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="25" t="s">
         <v>96</v>
-      </c>
-      <c r="H30" s="25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3453,10 +3546,10 @@
         <v>20 hours 9 minutes</v>
       </c>
       <c r="G31" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" s="25" t="s">
         <v>98</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3478,13 +3571,13 @@
         <v>23 hours 39 minutes</v>
       </c>
       <c r="G32" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="H32" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="27">
         <v>45220</v>
       </c>
@@ -3503,12 +3596,12 @@
         <v>0 hours 11 minutes</v>
       </c>
       <c r="G33" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>103</v>
       </c>
       <c r="B34" s="27">
         <v>45220</v>
@@ -3528,13 +3621,13 @@
         <v>2 hours 46 minutes</v>
       </c>
       <c r="G34" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="H34" s="25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="27">
         <v>45220</v>
       </c>
@@ -3553,13 +3646,13 @@
         <v>4 hours 46 minutes</v>
       </c>
       <c r="G35" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="H35" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="H35" s="25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="27">
         <v>45221</v>
       </c>
@@ -3578,13 +3671,13 @@
         <v>5 hours 36 minutes</v>
       </c>
       <c r="G36" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="H36" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="27">
         <v>45221</v>
       </c>
@@ -3603,13 +3696,13 @@
         <v>7 hours 11 minutes</v>
       </c>
       <c r="G37" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="H37" s="25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="27">
         <v>45223</v>
       </c>
@@ -3628,13 +3721,13 @@
         <v>11 hours 28 minutes</v>
       </c>
       <c r="G38" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="H38" s="25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B39" s="27">
         <v>45224</v>
       </c>
@@ -3653,13 +3746,13 @@
         <v>13 hours 36 minutes</v>
       </c>
       <c r="G39" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="H39" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="H39" s="25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="27">
         <v>45225</v>
       </c>
@@ -3678,10 +3771,10 @@
         <v>16 hours 1 minutes</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B41" s="27">
         <v>45226</v>
       </c>
@@ -3700,23 +3793,41 @@
         <v>20 hours 21 minutes</v>
       </c>
       <c r="G41" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="H41" s="25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E42" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B42" s="27">
+        <v>45227</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="E42" s="17">
+        <f t="shared" si="5"/>
+        <v>0.13541666666666663</v>
       </c>
       <c r="F42" s="15" t="str">
         <f>IF(E42="","",_xlfn.CONCAT(HOUR(SUM($E$4:E42))," hours ",MINUTE(SUM($E$4:E42))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23 hours 36 minutes</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="I42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3726,7 +3837,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3736,7 +3847,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3746,7 +3857,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3756,7 +3867,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E47" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -3766,7 +3877,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>

</xml_diff>

<commit_message>
messed with colors and project config frontend
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A7B393-C40F-43E8-A945-9B75C523A729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0B92D-FB23-4AB8-AAC7-9650C0A85D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="145">
   <si>
     <t>Start Time:</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Started the topbar frontend bits, created a new context hook for project metadata, changed how redirects work, also fixed auto sign out I think</t>
+  </si>
+  <si>
+    <t>messed with theme colors and project config frontend, fixed index button</t>
   </si>
 </sst>
 </file>
@@ -1468,8 +1471,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1932,7 @@
       </c>
       <c r="AK4" s="40" t="str">
         <f t="shared" si="3"/>
-        <v>03 hours 15 minutes</v>
+        <v>05 hours 05 minutes</v>
       </c>
       <c r="AL4" s="42" t="str">
         <f t="shared" si="3"/>
@@ -2515,171 +2518,171 @@
       </c>
       <c r="AK6" s="48" t="str" cm="1">
         <f t="array" ref="AK6">INT((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AK$4, 2))), SUM(MID($K$4:AK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>95 hours 36 minutes</v>
+        <v>97 hours 26 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3827,14 +3830,26 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E43" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="27">
+        <v>45227</v>
+      </c>
+      <c r="C43" s="16">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D43" s="12">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E43" s="17">
+        <f t="shared" si="5"/>
+        <v>7.638888888888884E-2</v>
       </c>
       <c r="F43" s="15" t="str">
         <f>IF(E43="","",_xlfn.CONCAT(HOUR(SUM($E$4:E43))," hours ",MINUTE(SUM($E$4:E43))," minutes"))</f>
-        <v/>
+        <v>1 hours 26 minutes</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lotsa frontend, auth pages, topbars, and saving
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E0B92D-FB23-4AB8-AAC7-9650C0A85D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D1281-FDAC-49C5-8CFF-77E781666DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="148">
   <si>
     <t>Start Time:</t>
   </si>
@@ -438,9 +438,6 @@
     <t>Next I want to finish the auto sign out, after that I think I wanna do the editor navbar and other editor things</t>
   </si>
   <si>
-    <t>77 hours</t>
-  </si>
-  <si>
     <t>82 hours</t>
   </si>
   <si>
@@ -493,6 +490,18 @@
   </si>
   <si>
     <t>messed with theme colors and project config frontend, fixed index button</t>
+  </si>
+  <si>
+    <t>Got the save button working, sonfig menu as well</t>
+  </si>
+  <si>
+    <t>78 hours</t>
+  </si>
+  <si>
+    <t>Merged the SignIn/Up pages and made them look real nice</t>
+  </si>
+  <si>
+    <t>Index and dashboard need work. Editor still needs some crucial buttons and the auto file display update</t>
   </si>
 </sst>
 </file>
@@ -1471,8 +1480,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +1945,7 @@
       </c>
       <c r="AL4" s="42" t="str">
         <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 20 minutes</v>
       </c>
       <c r="AM4" s="35" t="str">
         <f t="shared" si="3"/>
@@ -2226,10 +2235,10 @@
         <v>72</v>
       </c>
       <c r="AK5" s="44" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AL5" s="45" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="AM5" s="36" t="s">
         <v>16</v>
@@ -2522,167 +2531,167 @@
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>97 hours 26 minutes</v>
+        <v>100 hours 46 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2868,52 +2877,52 @@
         <v>85</v>
       </c>
       <c r="AK7" s="39" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="AL7" s="39" t="s">
         <v>86</v>
       </c>
       <c r="AM7" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN7" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="AN7" s="39" t="s">
+      <c r="AO7" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="AO7" s="39" t="s">
+      <c r="AP7" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="AP7" s="39" t="s">
+      <c r="AQ7" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="AQ7" s="39" t="s">
+      <c r="AR7" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="AR7" s="39" t="s">
+      <c r="AS7" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="AS7" s="39" t="s">
+      <c r="AT7" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="AT7" s="39" t="s">
+      <c r="AU7" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="AU7" s="39" t="s">
+      <c r="AV7" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="AV7" s="39" t="s">
+      <c r="AW7" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="AW7" s="39" t="s">
+      <c r="AX7" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="AX7" s="39" t="s">
+      <c r="AY7" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="AY7" s="39" t="s">
+      <c r="AZ7" s="39" t="s">
         <v>139</v>
-      </c>
-      <c r="AZ7" s="39" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
@@ -3821,13 +3830,13 @@
         <v>23 hours 36 minutes</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H42" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="I42" t="s">
         <v>141</v>
-      </c>
-      <c r="I42" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3849,27 +3858,54 @@
         <v>1 hours 26 minutes</v>
       </c>
       <c r="G43" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="27">
+        <v>45228</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="D44" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="E44" s="17">
+        <f t="shared" si="5"/>
+        <v>8.680555555555558E-2</v>
       </c>
       <c r="F44" s="15" t="str">
         <f>IF(E44="","",_xlfn.CONCAT(HOUR(SUM($E$4:E44))," hours ",MINUTE(SUM($E$4:E44))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>3 hours 31 minutes</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="27">
+        <v>45228</v>
+      </c>
+      <c r="C45" s="16">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D45" s="12">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="E45" s="17">
+        <f t="shared" si="5"/>
+        <v>5.2083333333333481E-2</v>
       </c>
       <c r="F45" s="15" t="str">
         <f>IF(E45="","",_xlfn.CONCAT(HOUR(SUM($E$4:E45))," hours ",MINUTE(SUM($E$4:E45))," minutes"))</f>
-        <v/>
+        <v>4 hours 46 minutes</v>
+      </c>
+      <c r="G45" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="H45" s="25" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Editor can now use EditorContext, commented logs
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D1281-FDAC-49C5-8CFF-77E781666DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507FFE9-74CB-4C4A-8E84-0941F1CC475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="148">
   <si>
     <t>Start Time:</t>
   </si>
@@ -498,10 +498,10 @@
     <t>78 hours</t>
   </si>
   <si>
-    <t>Merged the SignIn/Up pages and made them look real nice</t>
-  </si>
-  <si>
     <t>Index and dashboard need work. Editor still needs some crucial buttons and the auto file display update</t>
+  </si>
+  <si>
+    <t>Merged the SignIn/Up pages and made them look real nice, also refactored TopBar, then also fixed the part that I entirely broke</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1481,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="AL4" s="42" t="str">
         <f t="shared" si="3"/>
-        <v>03 hours 20 minutes</v>
+        <v>04 hours 05 minutes</v>
       </c>
       <c r="AM4" s="35" t="str">
         <f t="shared" si="3"/>
@@ -2531,167 +2531,167 @@
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>100 hours 46 minutes</v>
+        <v>101 hours 31 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3883,7 +3883,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="27">
         <v>45228</v>
       </c>
@@ -3891,21 +3891,21 @@
         <v>0.64236111111111105</v>
       </c>
       <c r="D45" s="12">
-        <v>0.69444444444444453</v>
+        <v>0.72569444444444453</v>
       </c>
       <c r="E45" s="17">
         <f t="shared" si="5"/>
-        <v>5.2083333333333481E-2</v>
+        <v>8.3333333333333481E-2</v>
       </c>
       <c r="F45" s="15" t="str">
         <f>IF(E45="","",_xlfn.CONCAT(HOUR(SUM($E$4:E45))," hours ",MINUTE(SUM($E$4:E45))," minutes"))</f>
-        <v>4 hours 46 minutes</v>
+        <v>5 hours 31 minutes</v>
       </c>
       <c r="G45" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="H45" s="25" t="s">
         <v>146</v>
-      </c>
-      <c r="H45" s="25" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
In the middle of typescript conversion
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507FFE9-74CB-4C4A-8E84-0941F1CC475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071D0951-E18E-4D0A-B50F-A5DED91B61E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="150">
   <si>
     <t>Start Time:</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>Merged the SignIn/Up pages and made them look real nice, also refactored TopBar, then also fixed the part that I entirely broke</t>
+  </si>
+  <si>
+    <t>Added Oauth buttons and started on the oauth backend logic</t>
+  </si>
+  <si>
+    <t>finish oauth</t>
   </si>
 </sst>
 </file>
@@ -1480,8 +1486,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +1951,7 @@
       </c>
       <c r="AL4" s="42" t="str">
         <f t="shared" si="3"/>
-        <v>04 hours 05 minutes</v>
+        <v>04 hours 20 minutes</v>
       </c>
       <c r="AM4" s="35" t="str">
         <f t="shared" si="3"/>
@@ -2531,167 +2537,167 @@
       </c>
       <c r="AL6" s="49" t="str" cm="1">
         <f t="array" ref="AL6">INT((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AL$4, 2))), SUM(MID($K$4:AL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AM6" s="46" t="str" cm="1">
         <f t="array" ref="AM6">INT((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AM$4, 2))), SUM(MID($K$4:AM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>101 hours 46 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3908,17 +3914,38 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="27">
+        <v>45228</v>
+      </c>
+      <c r="C46" s="16">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D46" s="12">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="E46" s="17">
+        <f t="shared" si="5"/>
+        <v>1.0416666666666741E-2</v>
       </c>
       <c r="F46" s="15" t="str">
         <f>IF(E46="","",_xlfn.CONCAT(HOUR(SUM($E$4:E46))," hours ",MINUTE(SUM($E$4:E46))," minutes"))</f>
-        <v/>
+        <v>5 hours 46 minutes</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="H46" s="25" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="27">
+        <v>45230</v>
+      </c>
+      <c r="C47" s="16">
+        <v>0.47569444444444442</v>
+      </c>
       <c r="E47" s="17" t="str">
         <f t="shared" si="5"/>
         <v/>

</xml_diff>

<commit_message>
So much, check excel spreadsheet at todays date
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507FFE9-74CB-4C4A-8E84-0941F1CC475E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1132041-8A3D-4AA8-A761-FC10E3E2DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="152">
   <si>
     <t>Start Time:</t>
   </si>
@@ -502,6 +503,18 @@
   </si>
   <si>
     <t>Merged the SignIn/Up pages and made them look real nice, also refactored TopBar, then also fixed the part that I entirely broke</t>
+  </si>
+  <si>
+    <t>Broke next.js hot reload, tweaked saving, starting on auto filestructure updating</t>
+  </si>
+  <si>
+    <t>Fixed the hot reload, got auto filestructuredisplay updating, started with the add file/folder button, fixed auto sign out, added some new fileOperations, fixed SharedArrayBuffer bug, improved saving and editor tabs</t>
+  </si>
+  <si>
+    <t>I didn't even mean to make up for my missed hours haha</t>
+  </si>
+  <si>
+    <t>Next is the new file/folder button functionality</t>
   </si>
 </sst>
 </file>
@@ -1480,8 +1493,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,6 +1550,9 @@
       </c>
       <c r="AM2" t="s">
         <v>106</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>150</v>
       </c>
       <c r="AT2" t="s">
         <v>107</v>
@@ -1836,15 +1852,15 @@
         <v>14</v>
       </c>
       <c r="K4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, K$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" ref="K4:AG4" si="0">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, K$3), "hh ""hours ""mm ""minutes""")</f>
         <v>01 hours 40 minutes</v>
       </c>
       <c r="L4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, L$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" si="0"/>
         <v>02 hours 53 minutes</v>
       </c>
       <c r="M4" s="35" t="str">
-        <f t="shared" ref="M4:Q4" si="0">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, M$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" si="0"/>
         <v>02 hours 20 minutes</v>
       </c>
       <c r="N4" s="35" t="str">
@@ -1864,247 +1880,247 @@
         <v>02 hours 38 minutes</v>
       </c>
       <c r="R4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, R$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" si="0"/>
         <v>03 hours 33 minutes</v>
       </c>
       <c r="S4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, S$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" si="0"/>
         <v>05 hours 50 minutes</v>
       </c>
       <c r="T4" s="35" t="str">
-        <f t="shared" ref="T4:X4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, T$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" si="0"/>
         <v>04 hours 23 minutes</v>
       </c>
       <c r="U4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>03 hours 35 minutes</v>
+      </c>
+      <c r="V4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>04 hours 35 minutes</v>
+      </c>
+      <c r="W4" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>07 hours 00 minutes</v>
+      </c>
+      <c r="X4" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>03 hours 25 minutes</v>
+      </c>
+      <c r="Y4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>03 hours 50 minutes</v>
+      </c>
+      <c r="Z4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>04 hours 10 minutes</v>
+      </c>
+      <c r="AA4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>02 hours 40 minutes</v>
+      </c>
+      <c r="AB4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>02 hours 21 minutes</v>
+      </c>
+      <c r="AC4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>03 hours 30 minutes</v>
+      </c>
+      <c r="AD4" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>05 hours 07 minutes</v>
+      </c>
+      <c r="AE4" s="42" t="str">
+        <f t="shared" si="0"/>
+        <v>02 hours 25 minutes</v>
+      </c>
+      <c r="AF4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>00 hours 00 minutes</v>
+      </c>
+      <c r="AG4" s="35" t="str">
+        <f t="shared" si="0"/>
+        <v>04 hours 17 minutes</v>
+      </c>
+      <c r="AH4" s="35" t="str">
+        <f t="shared" ref="AH4:BZ4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AH$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>02 hours 08 minutes</v>
+      </c>
+      <c r="AI4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>03 hours 35 minutes</v>
-      </c>
-      <c r="V4" s="35" t="str">
+        <v>02 hours 25 minutes</v>
+      </c>
+      <c r="AJ4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>04 hours 35 minutes</v>
-      </c>
-      <c r="W4" s="40" t="str">
+        <v>04 hours 20 minutes</v>
+      </c>
+      <c r="AK4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>07 hours 00 minutes</v>
-      </c>
-      <c r="X4" s="42" t="str">
+        <v>05 hours 05 minutes</v>
+      </c>
+      <c r="AL4" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>03 hours 25 minutes</v>
-      </c>
-      <c r="Y4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Y$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>03 hours 50 minutes</v>
-      </c>
-      <c r="Z4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, Z$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>04 hours 10 minutes</v>
-      </c>
-      <c r="AA4" s="35" t="str">
-        <f t="shared" ref="AA4:AE4" si="2">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AA$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>02 hours 40 minutes</v>
-      </c>
-      <c r="AB4" s="35" t="str">
-        <f t="shared" si="2"/>
-        <v>02 hours 21 minutes</v>
-      </c>
-      <c r="AC4" s="35" t="str">
-        <f t="shared" si="2"/>
-        <v>03 hours 30 minutes</v>
-      </c>
-      <c r="AD4" s="40" t="str">
-        <f t="shared" si="2"/>
-        <v>05 hours 07 minutes</v>
-      </c>
-      <c r="AE4" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>02 hours 25 minutes</v>
-      </c>
-      <c r="AF4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AF$3), "hh ""hours ""mm ""minutes""")</f>
+        <v>04 hours 05 minutes</v>
+      </c>
+      <c r="AM4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AG4" s="35" t="str">
-        <f>TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AG$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>04 hours 17 minutes</v>
-      </c>
-      <c r="AH4" s="35" t="str">
-        <f t="shared" ref="AH4:BZ4" si="3">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AH$3), "hh ""hours ""mm ""minutes""")</f>
-        <v>02 hours 08 minutes</v>
-      </c>
-      <c r="AI4" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>02 hours 25 minutes</v>
-      </c>
-      <c r="AJ4" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>04 hours 20 minutes</v>
-      </c>
-      <c r="AK4" s="40" t="str">
-        <f t="shared" si="3"/>
-        <v>05 hours 05 minutes</v>
-      </c>
-      <c r="AL4" s="42" t="str">
-        <f t="shared" si="3"/>
-        <v>04 hours 05 minutes</v>
-      </c>
-      <c r="AM4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AN4" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>06 hours 11 minutes</v>
+      </c>
+      <c r="AO4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AN4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AP4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AO4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AQ4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AP4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AR4" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AQ4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AS4" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AR4" s="40" t="str">
-        <f t="shared" si="3"/>
+      <c r="AT4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AS4" s="42" t="str">
-        <f t="shared" si="3"/>
+      <c r="AU4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AT4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AV4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AU4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AW4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AV4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AX4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AW4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AY4" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AX4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="AZ4" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AY4" s="40" t="str">
-        <f t="shared" si="3"/>
+      <c r="BA4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="AZ4" s="42" t="str">
-        <f t="shared" si="3"/>
+      <c r="BB4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BA4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BC4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BB4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BD4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BC4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BE4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BD4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BF4" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BE4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BG4" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BF4" s="40" t="str">
-        <f t="shared" si="3"/>
+      <c r="BH4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BG4" s="42" t="str">
-        <f t="shared" si="3"/>
+      <c r="BI4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BH4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BJ4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BI4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BK4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BJ4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BL4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BK4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BM4" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BL4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BN4" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BM4" s="40" t="str">
-        <f t="shared" si="3"/>
+      <c r="BO4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BN4" s="42" t="str">
-        <f t="shared" si="3"/>
+      <c r="BP4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BO4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BQ4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BP4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BR4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BQ4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BS4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BR4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BT4" s="40" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BS4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BU4" s="42" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BT4" s="40" t="str">
-        <f t="shared" si="3"/>
+      <c r="BV4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BU4" s="42" t="str">
-        <f t="shared" si="3"/>
+      <c r="BW4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BV4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BX4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BW4" s="35" t="str">
-        <f t="shared" si="3"/>
+      <c r="BY4" s="35" t="str">
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BX4" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
-      </c>
-      <c r="BY4" s="35" t="str">
-        <f t="shared" si="3"/>
-        <v>00 hours 00 minutes</v>
-      </c>
       <c r="BZ4" s="35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
       <c r="CA4" s="40"/>
@@ -2141,7 +2157,7 @@
         <v>0.82847222222222217</v>
       </c>
       <c r="E5" s="17">
-        <f t="shared" ref="E5" si="4">IF(OR(C5=0, D5=0),"", D5-C5)</f>
+        <f>IF(OR(C5=0, D5=0),"", D5-C5)</f>
         <v>0.1201388888888888</v>
       </c>
       <c r="F5" s="15" t="str">
@@ -2539,159 +2555,159 @@
       </c>
       <c r="AN6" s="37" t="str" cm="1">
         <f t="array" ref="AN6">INT((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AN$4, 2))), SUM(MID($K$4:AN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>101 hours 31 minutes</v>
+        <v>107 hours 42 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2779,7 +2795,7 @@
         <v>0.5180555555555556</v>
       </c>
       <c r="E7" s="17">
-        <f t="shared" ref="E7:E70" si="5">IF(OR(C7=0, D7=0),"", D7-C7)</f>
+        <f t="shared" ref="E7:E70" si="2">IF(OR(C7=0, D7=0),"", D7-C7)</f>
         <v>0.12222222222222229</v>
       </c>
       <c r="F7" s="15" t="str">
@@ -2936,7 +2952,7 @@
         <v>0.69097222222222221</v>
       </c>
       <c r="E8" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.16111111111111109</v>
       </c>
       <c r="F8" s="15" t="str">
@@ -2964,7 +2980,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="E9" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.18263888888888891</v>
       </c>
       <c r="F9" s="15" t="str">
@@ -2992,7 +3008,7 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="E10" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.6805555555555469E-2</v>
       </c>
       <c r="F10" s="15" t="str">
@@ -3048,7 +3064,7 @@
         <v>0.89444444444444438</v>
       </c>
       <c r="E12" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>5.0694444444444375E-2</v>
       </c>
       <c r="F12" s="15" t="str">
@@ -3076,7 +3092,7 @@
         <v>0.62847222222222221</v>
       </c>
       <c r="E13" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>1.736111111111116E-2</v>
       </c>
       <c r="F13" s="15" t="str">
@@ -3104,7 +3120,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="E14" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.13055555555555554</v>
       </c>
       <c r="F14" s="15" t="str">
@@ -3132,7 +3148,7 @@
         <v>0.5625</v>
       </c>
       <c r="E15" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.13541666666666669</v>
       </c>
       <c r="F15" s="15" t="str">
@@ -3149,7 +3165,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:151" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:151" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -3160,7 +3176,7 @@
         <v>0.80902777777777779</v>
       </c>
       <c r="E16" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.10763888888888895</v>
       </c>
       <c r="F16" s="15" t="str">
@@ -3185,7 +3201,7 @@
         <v>0.51388888888888895</v>
       </c>
       <c r="E17" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>9.3750000000000056E-2</v>
       </c>
       <c r="F17" s="15" t="str">
@@ -3207,7 +3223,7 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="E18" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.8888888888888906E-2</v>
       </c>
       <c r="F18" s="15" t="str">
@@ -3235,7 +3251,7 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E19" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7.6388888888888784E-2</v>
       </c>
       <c r="F19" s="15" t="str">
@@ -3291,7 +3307,7 @@
         <v>0.56597222222222221</v>
       </c>
       <c r="E21" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="F21" s="15" t="str">
@@ -3313,7 +3329,7 @@
         <v>0.90277777777777779</v>
       </c>
       <c r="E22" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7.986111111111116E-2</v>
       </c>
       <c r="F22" s="15" t="str">
@@ -3330,7 +3346,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>45213</v>
       </c>
@@ -3341,7 +3357,7 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="E23" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="F23" s="15" t="str">
@@ -3358,7 +3374,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>45214</v>
       </c>
@@ -3369,7 +3385,7 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="E24" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.14236111111111105</v>
       </c>
       <c r="F24" s="15" t="str">
@@ -3386,7 +3402,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
@@ -3397,7 +3413,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="E25" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.15972222222222232</v>
       </c>
       <c r="F25" s="15" t="str">
@@ -3425,7 +3441,7 @@
         <v>0.55902777777777779</v>
       </c>
       <c r="E26" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>9.027777777777779E-2</v>
       </c>
       <c r="F26" s="15" t="str">
@@ -3447,7 +3463,7 @@
         <v>0.66319444444444442</v>
       </c>
       <c r="E27" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F27" s="15" t="str">
@@ -3475,7 +3491,7 @@
         <v>0.76041666666666663</v>
       </c>
       <c r="E28" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.11111111111111105</v>
       </c>
       <c r="F28" s="15" t="str">
@@ -3500,7 +3516,7 @@
         <v>0.45902777777777781</v>
       </c>
       <c r="E29" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.5416666666666707E-2</v>
       </c>
       <c r="F29" s="15" t="str">
@@ -3525,7 +3541,7 @@
         <v>0.5625</v>
       </c>
       <c r="E30" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="F30" s="15" t="str">
@@ -3550,7 +3566,7 @@
         <v>0.66319444444444442</v>
       </c>
       <c r="E31" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F31" s="15" t="str">
@@ -3575,7 +3591,7 @@
         <v>0.625</v>
       </c>
       <c r="E32" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.14583333333333331</v>
       </c>
       <c r="F32" s="15" t="str">
@@ -3600,7 +3616,7 @@
         <v>0.52222222222222225</v>
       </c>
       <c r="E33" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>2.2222222222222254E-2</v>
       </c>
       <c r="F33" s="15" t="str">
@@ -3625,7 +3641,7 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="E34" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.10763888888888884</v>
       </c>
       <c r="F34" s="15" t="str">
@@ -3650,7 +3666,7 @@
         <v>0.79513888888888884</v>
       </c>
       <c r="E35" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="F35" s="15" t="str">
@@ -3675,7 +3691,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="E36" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>3.4722222222222154E-2</v>
       </c>
       <c r="F36" s="15" t="str">
@@ -3700,7 +3716,7 @@
         <v>0.89236111111111116</v>
       </c>
       <c r="E37" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>6.5972222222222321E-2</v>
       </c>
       <c r="F37" s="15" t="str">
@@ -3725,7 +3741,7 @@
         <v>0.84861111111111109</v>
       </c>
       <c r="E38" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.17847222222222225</v>
       </c>
       <c r="F38" s="15" t="str">
@@ -3750,7 +3766,7 @@
         <v>0.81805555555555554</v>
       </c>
       <c r="E39" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.8888888888888906E-2</v>
       </c>
       <c r="F39" s="15" t="str">
@@ -3775,7 +3791,7 @@
         <v>0.77777777777777779</v>
       </c>
       <c r="E40" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.10069444444444442</v>
       </c>
       <c r="F40" s="15" t="str">
@@ -3797,7 +3813,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="E41" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.18055555555555558</v>
       </c>
       <c r="F41" s="15" t="str">
@@ -3822,7 +3838,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="E42" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.13541666666666663</v>
       </c>
       <c r="F42" s="15" t="str">
@@ -3850,7 +3866,7 @@
         <v>0.84722222222222221</v>
       </c>
       <c r="E43" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>7.638888888888884E-2</v>
       </c>
       <c r="F43" s="15" t="str">
@@ -3872,7 +3888,7 @@
         <v>0.625</v>
       </c>
       <c r="E44" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.680555555555558E-2</v>
       </c>
       <c r="F44" s="15" t="str">
@@ -3894,7 +3910,7 @@
         <v>0.72569444444444453</v>
       </c>
       <c r="E45" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>8.3333333333333481E-2</v>
       </c>
       <c r="F45" s="15" t="str">
@@ -3908,29 +3924,56 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E46" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="27">
+        <v>45230</v>
+      </c>
+      <c r="C46" s="16">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D46" s="12">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="E46" s="17">
+        <f t="shared" si="2"/>
+        <v>0.1256944444444445</v>
       </c>
       <c r="F46" s="15" t="str">
         <f>IF(E46="","",_xlfn.CONCAT(HOUR(SUM($E$4:E46))," hours ",MINUTE(SUM($E$4:E46))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <v>8 hours 32 minutes</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B47" s="27">
+        <v>45230</v>
+      </c>
+      <c r="C47" s="16">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D47" s="12">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="E47" s="17">
+        <f t="shared" si="2"/>
+        <v>0.13194444444444453</v>
       </c>
       <c r="F47" s="15" t="str">
         <f>IF(E47="","",_xlfn.CONCAT(HOUR(SUM($E$4:E47))," hours ",MINUTE(SUM($E$4:E47))," minutes"))</f>
-        <v/>
+        <v>11 hours 42 minutes</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F48" s="15" t="str">
@@ -3940,7 +3983,7 @@
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E49" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F49" s="15" t="str">
@@ -3950,7 +3993,7 @@
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F50" s="15" t="str">
@@ -3960,7 +4003,7 @@
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E51" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F51" s="15" t="str">
@@ -3970,7 +4013,7 @@
     </row>
     <row r="52" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E52" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F52" s="15" t="str">
@@ -3980,7 +4023,7 @@
     </row>
     <row r="53" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E53" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F53" s="15" t="str">
@@ -3990,7 +4033,7 @@
     </row>
     <row r="54" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E54" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F54" s="15" t="str">
@@ -4000,7 +4043,7 @@
     </row>
     <row r="55" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E55" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F55" s="15" t="str">
@@ -4010,7 +4053,7 @@
     </row>
     <row r="56" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E56" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F56" s="15" t="str">
@@ -4020,7 +4063,7 @@
     </row>
     <row r="57" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E57" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F57" s="15" t="str">
@@ -4030,7 +4073,7 @@
     </row>
     <row r="58" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E58" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F58" s="15" t="str">
@@ -4040,7 +4083,7 @@
     </row>
     <row r="59" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E59" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F59" s="15" t="str">
@@ -4050,7 +4093,7 @@
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E60" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F60" s="15" t="str">
@@ -4060,7 +4103,7 @@
     </row>
     <row r="61" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E61" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F61" s="15" t="str">
@@ -4070,7 +4113,7 @@
     </row>
     <row r="62" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E62" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F62" s="15" t="str">
@@ -4080,7 +4123,7 @@
     </row>
     <row r="63" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E63" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F63" s="15" t="str">
@@ -4090,7 +4133,7 @@
     </row>
     <row r="64" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E64" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F64" s="15" t="str">
@@ -4100,7 +4143,7 @@
     </row>
     <row r="65" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E65" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F65" s="15" t="str">
@@ -4110,7 +4153,7 @@
     </row>
     <row r="66" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E66" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F66" s="15" t="str">
@@ -4120,7 +4163,7 @@
     </row>
     <row r="67" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E67" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F67" s="15" t="str">
@@ -4130,7 +4173,7 @@
     </row>
     <row r="68" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E68" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F68" s="15" t="str">
@@ -4140,7 +4183,7 @@
     </row>
     <row r="69" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E69" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F69" s="15" t="str">
@@ -4150,7 +4193,7 @@
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" s="17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F70" s="15" t="str">
@@ -4160,7 +4203,7 @@
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" s="17" t="str">
-        <f t="shared" ref="E71:E125" si="6">IF(OR(C71=0, D71=0),"", D71-C71)</f>
+        <f t="shared" ref="E71:E125" si="3">IF(OR(C71=0, D71=0),"", D71-C71)</f>
         <v/>
       </c>
       <c r="F71" s="15" t="str">
@@ -4170,7 +4213,7 @@
     </row>
     <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F72" s="15" t="str">
@@ -4180,7 +4223,7 @@
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F73" s="15" t="str">
@@ -4190,7 +4233,7 @@
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F74" s="15" t="str">
@@ -4200,7 +4243,7 @@
     </row>
     <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E75" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F75" s="15" t="str">
@@ -4210,7 +4253,7 @@
     </row>
     <row r="76" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E76" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F76" s="15" t="str">
@@ -4220,7 +4263,7 @@
     </row>
     <row r="77" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E77" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F77" s="15" t="str">
@@ -4230,7 +4273,7 @@
     </row>
     <row r="78" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E78" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F78" s="15" t="str">
@@ -4240,7 +4283,7 @@
     </row>
     <row r="79" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E79" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F79" s="15" t="str">
@@ -4250,7 +4293,7 @@
     </row>
     <row r="80" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E80" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F80" s="15" t="str">
@@ -4260,7 +4303,7 @@
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F81" s="15" t="str">
@@ -4270,7 +4313,7 @@
     </row>
     <row r="82" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E82" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F82" s="15" t="str">
@@ -4280,7 +4323,7 @@
     </row>
     <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F83" s="15" t="str">
@@ -4290,7 +4333,7 @@
     </row>
     <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E84" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F84" s="15" t="str">
@@ -4300,7 +4343,7 @@
     </row>
     <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F85" s="15" t="str">
@@ -4310,7 +4353,7 @@
     </row>
     <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F86" s="15" t="str">
@@ -4320,7 +4363,7 @@
     </row>
     <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F87" s="15" t="str">
@@ -4330,7 +4373,7 @@
     </row>
     <row r="88" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E88" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F88" s="15" t="str">
@@ -4340,7 +4383,7 @@
     </row>
     <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F89" s="15" t="str">
@@ -4350,7 +4393,7 @@
     </row>
     <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E90" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F90" s="15" t="str">
@@ -4360,7 +4403,7 @@
     </row>
     <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F91" s="15" t="str">
@@ -4370,7 +4413,7 @@
     </row>
     <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F92" s="15" t="str">
@@ -4380,7 +4423,7 @@
     </row>
     <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F93" s="15" t="str">
@@ -4390,7 +4433,7 @@
     </row>
     <row r="94" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E94" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F94" s="15" t="str">
@@ -4400,7 +4443,7 @@
     </row>
     <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F95" s="15" t="str">
@@ -4410,7 +4453,7 @@
     </row>
     <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E96" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F96" s="15" t="str">
@@ -4420,7 +4463,7 @@
     </row>
     <row r="97" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E97" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F97" s="15" t="str">
@@ -4430,7 +4473,7 @@
     </row>
     <row r="98" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E98" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F98" s="15" t="str">
@@ -4440,7 +4483,7 @@
     </row>
     <row r="99" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E99" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F99" s="15" t="str">
@@ -4450,7 +4493,7 @@
     </row>
     <row r="100" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E100" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F100" s="15" t="str">
@@ -4460,7 +4503,7 @@
     </row>
     <row r="101" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E101" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F101" s="15" t="str">
@@ -4470,7 +4513,7 @@
     </row>
     <row r="102" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E102" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F102" s="15" t="str">
@@ -4480,7 +4523,7 @@
     </row>
     <row r="103" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E103" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F103" s="15" t="str">
@@ -4490,7 +4533,7 @@
     </row>
     <row r="104" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E104" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F104" s="15" t="str">
@@ -4500,7 +4543,7 @@
     </row>
     <row r="105" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E105" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="F105" s="15" t="str">
@@ -4510,121 +4553,121 @@
     </row>
     <row r="106" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E106" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="107" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E107" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="108" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E108" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="109" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E109" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="110" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E110" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="111" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E111" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="112" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E112" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Styling and file/folder name validation
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1132041-8A3D-4AA8-A761-FC10E3E2DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6939FC90-7EB4-49A5-B596-A21CD66F8046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
     <t>Start Time:</t>
   </si>
@@ -515,6 +514,12 @@
   </si>
   <si>
     <t>Next is the new file/folder button functionality</t>
+  </si>
+  <si>
+    <t>Styling and file/folder name validation</t>
+  </si>
+  <si>
+    <t>^^^^^^^^^^^^</t>
   </si>
 </sst>
 </file>
@@ -1494,7 +1499,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1978,7 @@
       </c>
       <c r="AO4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 15 minutes</v>
       </c>
       <c r="AP4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2559,155 +2564,155 @@
       </c>
       <c r="AO6" s="37" t="str" cm="1">
         <f t="array" ref="AO6">INT((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AO$4, 2))), SUM(MID($K$4:AO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AP6" s="37" t="str" cm="1">
         <f t="array" ref="AP6">INT((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AP$4, 2))), SUM(MID($K$4:AP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AQ6" s="47" t="str" cm="1">
         <f t="array" ref="AQ6">INT((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AQ$4, 2))), SUM(MID($K$4:AQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>107 hours 42 minutes</v>
+        <v>109 hours 57 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3402,7 +3407,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
@@ -3972,13 +3977,28 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E48" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B48" s="27">
+        <v>45231</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D48" s="12">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="E48" s="17">
+        <f t="shared" si="2"/>
+        <v>9.375E-2</v>
       </c>
       <c r="F48" s="15" t="str">
         <f>IF(E48="","",_xlfn.CONCAT(HOUR(SUM($E$4:E48))," hours ",MINUTE(SUM($E$4:E48))," minutes"))</f>
-        <v/>
+        <v>13 hours 57 minutes</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some stuff, check spreadsheet
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B31EDA-EB1B-498E-81DD-BE711F438F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A7E78F-F81E-4D13-9FB7-E9DC33A58F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
   <si>
     <t>Start Time:</t>
   </si>
@@ -532,6 +532,15 @@
   </si>
   <si>
     <t>Delete Files, diff button, fork button, profile viewer/search</t>
+  </si>
+  <si>
+    <t>Delete folders and files woohoo!</t>
+  </si>
+  <si>
+    <t>Reworked dashboard looks, added the profile view to it. Also made but didn not test the search for user endpoint, and made the get projects endpoints sort by last modified date</t>
+  </si>
+  <si>
+    <t>Next is making the profile viewer/editor actually update the profile, and add the profile collaborator components to the editor</t>
   </si>
 </sst>
 </file>
@@ -1510,8 +1519,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2011,7 @@
       </c>
       <c r="AR4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>00 hours 10 minutes</v>
       </c>
       <c r="AS4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -2010,7 +2019,7 @@
       </c>
       <c r="AT4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 07 minutes</v>
       </c>
       <c r="AU4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2588,143 +2597,143 @@
       </c>
       <c r="AR6" s="48" t="str" cm="1">
         <f t="array" ref="AR6">INT((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AR$4, 2))), SUM(MID($K$4:AR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>117 hours 47 minutes</v>
       </c>
       <c r="AS6" s="49" t="str" cm="1">
         <f t="array" ref="AS6">INT((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AS$4, 2))), SUM(MID($K$4:AS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>117 hours 47 minutes</v>
       </c>
       <c r="AT6" s="46" t="str" cm="1">
         <f t="array" ref="AT6">INT((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AT$4, 2))), SUM(MID($K$4:AT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>117 hours 37 minutes</v>
+        <v>119 hours 54 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4064,23 +4073,50 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E51" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B51" s="27">
+        <v>45234</v>
+      </c>
+      <c r="C51" s="16">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D51" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E51" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="F51" s="15" t="str">
         <f>IF(E51="","",_xlfn.CONCAT(HOUR(SUM($E$4:E51))," hours ",MINUTE(SUM($E$4:E51))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E52" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>21 hours 47 minutes</v>
+      </c>
+      <c r="G51" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B52" s="27">
+        <v>45236</v>
+      </c>
+      <c r="C52" s="16">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0.80833333333333324</v>
+      </c>
+      <c r="E52" s="17">
+        <f t="shared" si="2"/>
+        <v>8.8194444444444242E-2</v>
       </c>
       <c r="F52" s="15" t="str">
         <f>IF(E52="","",_xlfn.CONCAT(HOUR(SUM($E$4:E52))," hours ",MINUTE(SUM($E$4:E52))," minutes"))</f>
-        <v/>
+        <v>23 hours 54 minutes</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="H52" s="25" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
profile accordions, and profile editing
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A7E78F-F81E-4D13-9FB7-E9DC33A58F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB079084-7FE5-4137-B403-F154A59D6D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="164">
   <si>
     <t>Start Time:</t>
   </si>
@@ -541,6 +541,15 @@
   </si>
   <si>
     <t>Next is making the profile viewer/editor actually update the profile, and add the profile collaborator components to the editor</t>
+  </si>
+  <si>
+    <t>Need to make a public account view</t>
+  </si>
+  <si>
+    <t>Made the profile component on the dashboard update profiles, added profile accordions to the project config in the editor</t>
+  </si>
+  <si>
+    <t>Next is making the add and remove collaborator functions, right now the component is just pretty frontend</t>
   </si>
 </sst>
 </file>
@@ -1519,8 +1528,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2032,7 @@
       </c>
       <c r="AU4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 00 minutes</v>
       </c>
       <c r="AV4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2609,131 +2618,131 @@
       </c>
       <c r="AU6" s="37" t="str" cm="1">
         <f t="array" ref="AU6">INT((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AU$4, 2))), SUM(MID($K$4:AU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="AV6" s="37" t="str" cm="1">
         <f t="array" ref="AV6">INT((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AV$4, 2))), SUM(MID($K$4:AV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>119 hours 54 minutes</v>
+        <v>121 hours 54 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4022,7 +4031,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B49" s="27">
         <v>45232</v>
       </c>
@@ -4047,7 +4056,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="27">
         <v>45233</v>
       </c>
@@ -4072,7 +4081,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="27">
         <v>45234</v>
       </c>
@@ -4094,7 +4103,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" s="27">
         <v>45236</v>
       </c>
@@ -4119,17 +4128,35 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E53" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="53" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B53" s="27">
+        <v>45237</v>
+      </c>
+      <c r="C53" s="16">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D53" s="12">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E53" s="17">
+        <f t="shared" si="2"/>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="F53" s="15" t="str">
         <f>IF(E53="","",_xlfn.CONCAT(HOUR(SUM($E$4:E53))," hours ",MINUTE(SUM($E$4:E53))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+        <v>1 hours 54 minutes</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="I53" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E54" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4139,7 +4166,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E55" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4149,7 +4176,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E56" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4159,7 +4186,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E57" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4169,7 +4196,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E58" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4179,7 +4206,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E59" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4189,7 +4216,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E60" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4199,7 +4226,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E61" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4209,7 +4236,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E62" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4219,7 +4246,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E63" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4229,7 +4256,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E64" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>

</xml_diff>

<commit_message>
styles, template previews, diff editor
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B9460A-98BE-4F02-8141-F5CCB1878716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E49BB0-8E4C-4A0D-A1D6-ED7263C4243F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="168">
   <si>
     <t>Start Time:</t>
   </si>
@@ -552,10 +552,16 @@
     <t>Next is making the add and remove collaborator functions, right now the component is just pretty frontend</t>
   </si>
   <si>
-    <t>I got the collaborator stuff working! Collaborators can see shared projects on their dashboard, as well as update projects shared with them!</t>
-  </si>
-  <si>
     <t>I don't know what in particular to do next, but I know the diff button needs work still lol</t>
+  </si>
+  <si>
+    <t>I got the collaborator stuff working! Collaborators can see shared projects on their dashboard, as well as update projects shared with them! Oh also custom scrollbars in some places</t>
+  </si>
+  <si>
+    <t>Diff button finally implemented!!!! Mini File Display for the template preview on create project is implemented!! Started reworking the landing page!</t>
+  </si>
+  <si>
+    <t>Next is the public profile page/endpoints, as well as finishing up the landing page</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1540,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2052,7 @@
       </c>
       <c r="AW4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 25 minutes</v>
       </c>
       <c r="AX4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2632,123 +2638,123 @@
       </c>
       <c r="AW6" s="37" t="str" cm="1">
         <f t="array" ref="AW6">INT((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AW$4, 2))), SUM(MID($K$4:AW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>124 hours 34 minutes</v>
+        <v>126 hours 59 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4162,7 +4168,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B54" s="27">
         <v>45238</v>
       </c>
@@ -4181,20 +4187,35 @@
         <v>4 hours 34 minutes</v>
       </c>
       <c r="G54" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="H54" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="H54" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E55" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    </row>
+    <row r="55" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B55" s="27">
+        <v>45239</v>
+      </c>
+      <c r="C55" s="16">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="D55" s="12">
+        <v>0.8125</v>
+      </c>
+      <c r="E55" s="17">
+        <f t="shared" si="2"/>
+        <v>0.10069444444444453</v>
       </c>
       <c r="F55" s="15" t="str">
         <f>IF(E55="","",_xlfn.CONCAT(HOUR(SUM($E$4:E55))," hours ",MINUTE(SUM($E$4:E55))," minutes"))</f>
-        <v/>
+        <v>6 hours 59 minutes</v>
+      </c>
+      <c r="G55" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="H55" s="25" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Forking, tweaks, and fixes
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADA99AE-DF03-4EAA-9ADC-9A42C651BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BF7C69-E888-4EE9-8AB1-A509ADD9D81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
   <si>
     <t>Start Time:</t>
   </si>
@@ -568,6 +568,12 @@
   </si>
   <si>
     <t>Show off to Canterra</t>
+  </si>
+  <si>
+    <t>Dependency viewer, some bugs, the fork function, and more tweaks</t>
+  </si>
+  <si>
+    <t>Oauth or GPT stuff</t>
   </si>
 </sst>
 </file>
@@ -1546,8 +1552,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2068,7 @@
       </c>
       <c r="AX4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 40 minutes</v>
+        <v>03 hours 15 minutes</v>
       </c>
       <c r="AY4" s="40" t="str">
         <f t="shared" si="1"/>
@@ -2648,119 +2654,119 @@
       </c>
       <c r="AX6" s="47" t="str" cm="1">
         <f t="array" ref="AX6">INT((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AX$4, 2))), SUM(MID($K$4:AX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>127 hours 39 minutes</v>
+        <v>130 hours 13.9999999999991 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4249,14 +4255,29 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E57" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="57" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B57" s="27">
+        <v>45240</v>
+      </c>
+      <c r="C57" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="D57" s="12">
+        <v>0.73263888888888884</v>
+      </c>
+      <c r="E57" s="17">
+        <f t="shared" si="2"/>
+        <v>0.10763888888888884</v>
       </c>
       <c r="F57" s="15" t="str">
         <f>IF(E57="","",_xlfn.CONCAT(HOUR(SUM($E$4:E57))," hours ",MINUTE(SUM($E$4:E57))," minutes"))</f>
-        <v/>
+        <v>10 hours 14 minutes</v>
+      </c>
+      <c r="G57" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="25" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
multiday commit, gpt refactors, toasts, bugsquish
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BF7C69-E888-4EE9-8AB1-A509ADD9D81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23F6738-D481-47AF-9838-C865FDEBCEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="193">
   <si>
     <t>Start Time:</t>
   </si>
@@ -574,6 +574,69 @@
   </si>
   <si>
     <t>Oauth or GPT stuff</t>
+  </si>
+  <si>
+    <t>Big learning hours. Openai released a new beta feature that I will be implementing, it took me a minute to grasp how it works, but it actually works how I originally thought completions would</t>
+  </si>
+  <si>
+    <t>Next is to actually implement the new GPT chat functionality</t>
+  </si>
+  <si>
+    <t>Work on updating GPT chat functionality</t>
+  </si>
+  <si>
+    <t>122 hours</t>
+  </si>
+  <si>
+    <t>126 hours</t>
+  </si>
+  <si>
+    <t>128 hours</t>
+  </si>
+  <si>
+    <t>130 hours</t>
+  </si>
+  <si>
+    <t>133 hours</t>
+  </si>
+  <si>
+    <t>140 hours</t>
+  </si>
+  <si>
+    <t>138 hours</t>
+  </si>
+  <si>
+    <t>142 hours</t>
+  </si>
+  <si>
+    <t>146 hours</t>
+  </si>
+  <si>
+    <t>148 hours</t>
+  </si>
+  <si>
+    <t>150 hours</t>
+  </si>
+  <si>
+    <t>153 hours</t>
+  </si>
+  <si>
+    <t>158 hours</t>
+  </si>
+  <si>
+    <t>160 hours</t>
+  </si>
+  <si>
+    <t>Added toasts</t>
+  </si>
+  <si>
+    <t>That stuff ^^^^</t>
+  </si>
+  <si>
+    <t>Refactored GPT conversation stuff</t>
+  </si>
+  <si>
+    <t>Make it so you can change a projects start server command, that way we can support other project types</t>
   </si>
 </sst>
 </file>
@@ -1552,8 +1615,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2135,7 @@
       </c>
       <c r="AY4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 46 minutes</v>
       </c>
       <c r="AZ4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -2080,7 +2143,7 @@
       </c>
       <c r="BA4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 13 minutes</v>
       </c>
       <c r="BB4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2088,7 +2151,7 @@
       </c>
       <c r="BC4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 55 minutes</v>
       </c>
       <c r="BD4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2658,115 +2721,115 @@
       </c>
       <c r="AY6" s="48" t="str" cm="1">
         <f t="array" ref="AY6">INT((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AY$4, 2))), SUM(MID($K$4:AY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>133 hours 0 minutes</v>
       </c>
       <c r="AZ6" s="49" t="str" cm="1">
         <f t="array" ref="AZ6">INT((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:AZ$4, 2))), SUM(MID($K$4:AZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>133 hours 0 minutes</v>
       </c>
       <c r="BA6" s="46" t="str" cm="1">
         <f t="array" ref="BA6">INT((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BA$4, 2))), SUM(MID($K$4:BA$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>134 hours 13 minutes</v>
       </c>
       <c r="BB6" s="37" t="str" cm="1">
         <f t="array" ref="BB6">INT((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BB$4, 2))), SUM(MID($K$4:BB$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>134 hours 13 minutes</v>
       </c>
       <c r="BC6" s="37" t="str" cm="1">
         <f t="array" ref="BC6">INT((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BC$4, 2))), SUM(MID($K$4:BC$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>130 hours 13.9999999999991 minutes</v>
+        <v>137 hours 8 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2999,6 +3062,48 @@
       <c r="AZ7" s="39" t="s">
         <v>139</v>
       </c>
+      <c r="BA7" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="BB7" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="BC7" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD7" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="BE7" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="BF7" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="BG7" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="BH7" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="BI7" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="BJ7" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="BK7" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="BL7" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="BM7" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="BN7" s="39" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
@@ -3224,7 +3329,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:151" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:151" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -3405,7 +3510,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>45213</v>
       </c>
@@ -3433,7 +3538,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>45214</v>
       </c>
@@ -4280,44 +4385,101 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E58" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="58" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="B58" s="27">
+        <v>45241</v>
+      </c>
+      <c r="C58" s="16">
+        <v>0.59375</v>
+      </c>
+      <c r="D58" s="12">
+        <v>0.7090277777777777</v>
+      </c>
+      <c r="E58" s="17">
+        <f t="shared" si="2"/>
+        <v>0.1152777777777777</v>
       </c>
       <c r="F58" s="15" t="str">
         <f>IF(E58="","",_xlfn.CONCAT(HOUR(SUM($E$4:E58))," hours ",MINUTE(SUM($E$4:E58))," minutes"))</f>
-        <v/>
+        <v>13 hours 0 minutes</v>
+      </c>
+      <c r="G58" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="H58" s="25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E59" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B59" s="27">
+        <v>45243</v>
+      </c>
+      <c r="C59" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D59" s="12">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="E59" s="17">
+        <f t="shared" si="2"/>
+        <v>5.0694444444444431E-2</v>
       </c>
       <c r="F59" s="15" t="str">
         <f>IF(E59="","",_xlfn.CONCAT(HOUR(SUM($E$4:E59))," hours ",MINUTE(SUM($E$4:E59))," minutes"))</f>
-        <v/>
+        <v>14 hours 13 minutes</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E60" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="B60" s="27">
+        <v>45245</v>
+      </c>
+      <c r="C60" s="16">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D60" s="12">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="E60" s="17">
+        <f t="shared" si="2"/>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="F60" s="15" t="str">
         <f>IF(E60="","",_xlfn.CONCAT(HOUR(SUM($E$4:E60))," hours ",MINUTE(SUM($E$4:E60))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E61" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>15 hours 28 minutes</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="H60" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="27">
+        <v>45245</v>
+      </c>
+      <c r="C61" s="16">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D61" s="12">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="E61" s="17">
+        <f t="shared" si="2"/>
+        <v>6.9444444444444309E-2</v>
       </c>
       <c r="F61" s="15" t="str">
         <f>IF(E61="","",_xlfn.CONCAT(HOUR(SUM($E$4:E61))," hours ",MINUTE(SUM($E$4:E61))," minutes"))</f>
-        <v/>
+        <v>17 hours 8 minutes</v>
+      </c>
+      <c r="G61" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="H61" s="25" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Custom start command and profile tweaks
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23F6738-D481-47AF-9838-C865FDEBCEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EE244-7C37-493F-AA11-A1B8A2123E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="194">
   <si>
     <t>Start Time:</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>Make it so you can change a projects start server command, that way we can support other project types</t>
+  </si>
+  <si>
+    <t>You can change the projects start command now. Tweaked profile accordion</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1619,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,7 +2158,7 @@
       </c>
       <c r="BD4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 15 minutes</v>
       </c>
       <c r="BE4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2741,95 +2744,95 @@
       </c>
       <c r="BD6" s="37" t="str" cm="1">
         <f t="array" ref="BD6">INT((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BD$4, 2))), SUM(MID($K$4:BD$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>137 hours 8 minutes</v>
+        <v>138 hours 23 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4482,14 +4485,26 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E62" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="62" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="27">
+        <v>45246</v>
+      </c>
+      <c r="C62" s="16">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D62" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E62" s="17">
+        <f t="shared" si="2"/>
+        <v>5.2083333333333315E-2</v>
       </c>
       <c r="F62" s="15" t="str">
         <f>IF(E62="","",_xlfn.CONCAT(HOUR(SUM($E$4:E62))," hours ",MINUTE(SUM($E$4:E62))," minutes"))</f>
-        <v/>
+        <v>18 hours 23 minutes</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Download, frontpage work started not ended
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EE244-7C37-493F-AA11-A1B8A2123E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36720E27-DD37-4CC5-B8A2-C96F0716D132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="196">
   <si>
     <t>Start Time:</t>
   </si>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <t>You can change the projects start command now. Tweaked profile accordion</t>
+  </si>
+  <si>
+    <t>You can now download your projects, and I've started on the front page rework.</t>
+  </si>
+  <si>
+    <t>Continue the front page rework, after that is testing/polish/presentation prep</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1625,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,7 +2168,7 @@
       </c>
       <c r="BE4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 40 minutes</v>
       </c>
       <c r="BF4" s="40" t="str">
         <f t="shared" si="1"/>
@@ -2748,91 +2754,91 @@
       </c>
       <c r="BE6" s="47" t="str" cm="1">
         <f t="array" ref="BE6">INT((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BE$4, 2))), SUM(MID($K$4:BE$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>138 hours 23 minutes</v>
+        <v>142 hours 3 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4507,14 +4513,29 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E63" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="63" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="27">
+        <v>45247</v>
+      </c>
+      <c r="C63" s="16">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D63" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E63" s="17">
+        <f t="shared" si="2"/>
+        <v>0.15277777777777768</v>
       </c>
       <c r="F63" s="15" t="str">
         <f>IF(E63="","",_xlfn.CONCAT(HOUR(SUM($E$4:E63))," hours ",MINUTE(SUM($E$4:E63))," minutes"))</f>
-        <v/>
+        <v>22 hours 3 minutes</v>
+      </c>
+      <c r="G63" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="H63" s="25" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished mock editor, started next part of index
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36720E27-DD37-4CC5-B8A2-C96F0716D132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EC181D-8876-4C50-AA96-F0B591C5037B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="199">
   <si>
     <t>Start Time:</t>
   </si>
@@ -646,6 +646,15 @@
   </si>
   <si>
     <t>Continue the front page rework, after that is testing/polish/presentation prep</t>
+  </si>
+  <si>
+    <t>Finished up the mock editor, started on the next bit of the landing page</t>
+  </si>
+  <si>
+    <t>Landing page progress, get more of it done so you can work on GPT improvements or getting the project online</t>
+  </si>
+  <si>
+    <t>Another day to address unaddressed comments and spreadsheet items should be soon</t>
   </si>
 </sst>
 </file>
@@ -1624,8 +1633,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,7 +2181,7 @@
       </c>
       <c r="BF4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>03 hours 05 minutes</v>
       </c>
       <c r="BG4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -2758,87 +2767,87 @@
       </c>
       <c r="BF6" s="48" t="str" cm="1">
         <f t="array" ref="BF6">INT((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BF$4, 2))), SUM(MID($K$4:BF$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BG6" s="49" t="str" cm="1">
         <f t="array" ref="BG6">INT((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BG$4, 2))), SUM(MID($K$4:BG$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BH6" s="46" t="str" cm="1">
         <f t="array" ref="BH6">INT((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BH$4, 2))), SUM(MID($K$4:BH$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>142 hours 3 minutes</v>
+        <v>145 hours 8 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4538,17 +4547,32 @@
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E64" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="64" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B64" s="27">
+        <v>45248</v>
+      </c>
+      <c r="C64" s="16">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D64" s="12">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E64" s="17">
+        <f t="shared" si="2"/>
+        <v>0.12847222222222232</v>
       </c>
       <c r="F64" s="15" t="str">
         <f>IF(E64="","",_xlfn.CONCAT(HOUR(SUM($E$4:E64))," hours ",MINUTE(SUM($E$4:E64))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+        <v>1 hours 8 minutes</v>
+      </c>
+      <c r="G64" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="H64" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E65" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4558,7 +4582,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E66" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4567,8 +4591,11 @@
         <f>IF(E66="","",_xlfn.CONCAT(HOUR(SUM($E$4:E66))," hours ",MINUTE(SUM($E$4:E66))," minutes"))</f>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E67" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4578,7 +4605,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E68" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4588,7 +4615,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E69" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4598,7 +4625,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E70" s="17" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -4608,7 +4635,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E71" s="17" t="str">
         <f t="shared" ref="E71:E125" si="3">IF(OR(C71=0, D71=0),"", D71-C71)</f>
         <v/>
@@ -4618,7 +4645,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E72" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4628,7 +4655,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E73" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4638,7 +4665,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E74" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4648,7 +4675,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E75" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4658,7 +4685,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E76" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4668,7 +4695,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E77" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4678,7 +4705,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E78" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4688,7 +4715,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E79" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4698,7 +4725,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E80" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>

</xml_diff>

<commit_message>
Next.js in webbie as well as the empty project
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60C9748-C8CF-48C4-8878-7E1020B26E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD7185E-193A-417F-BBC3-1274A4C4F05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="205">
   <si>
     <t>Start Time:</t>
   </si>
@@ -661,6 +661,18 @@
   </si>
   <si>
     <t>Next is the "These frameworks are possible" blurb, which means testing/making templates for other project types, also the "No really try it" blurb and the footer need work</t>
+  </si>
+  <si>
+    <t>Got the blank template working and smoothed out some webContainer wrinkles, got stuck trying to get next.js running in the web container</t>
+  </si>
+  <si>
+    <t>Get next.js running in the web container, or move on to another node.js example/template.</t>
+  </si>
+  <si>
+    <t>Got unstuck! By switching to babel webpack</t>
+  </si>
+  <si>
+    <t>Next web framework!</t>
   </si>
 </sst>
 </file>
@@ -1639,8 +1651,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,11 +2211,11 @@
       </c>
       <c r="BI4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 55 minutes</v>
       </c>
       <c r="BJ4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>00 hours 40 minutes</v>
       </c>
       <c r="BK4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2785,75 +2797,75 @@
       </c>
       <c r="BI6" s="37" t="str" cm="1">
         <f t="array" ref="BI6">INT((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BI$4, 2))), SUM(MID($K$4:BI$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 13 minutes</v>
       </c>
       <c r="BJ6" s="37" t="str" cm="1">
         <f t="array" ref="BJ6">INT((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BJ$4, 2))), SUM(MID($K$4:BJ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BK6" s="37" t="str" cm="1">
         <f t="array" ref="BK6">INT((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BK$4, 2))), SUM(MID($K$4:BK$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>147 hours 18 minutes</v>
+        <v>150 hours 53 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4603,27 +4615,54 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E66" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="66" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B66" s="27">
+        <v>45251</v>
+      </c>
+      <c r="C66" s="16">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D66" s="12">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E66" s="17">
+        <f t="shared" si="2"/>
+        <v>0.12152777777777768</v>
       </c>
       <c r="F66" s="15" t="str">
         <f>IF(E66="","",_xlfn.CONCAT(HOUR(SUM($E$4:E66))," hours ",MINUTE(SUM($E$4:E66))," minutes"))</f>
-        <v/>
-      </c>
-      <c r="I66" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E67" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>6 hours 13 minutes</v>
+      </c>
+      <c r="G66" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H66" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B67" s="27">
+        <v>45252</v>
+      </c>
+      <c r="C67" s="16">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D67" s="12">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E67" s="17">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777735E-2</v>
       </c>
       <c r="F67" s="15" t="str">
         <f>IF(E67="","",_xlfn.CONCAT(HOUR(SUM($E$4:E67))," hours ",MINUTE(SUM($E$4:E67))," minutes"))</f>
-        <v/>
+        <v>6 hours 53 minutes</v>
+      </c>
+      <c r="G67" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H67" s="25" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
@@ -4644,6 +4683,9 @@
       <c r="F69" s="15" t="str">
         <f>IF(E69="","",_xlfn.CONCAT(HOUR(SUM($E$4:E69))," hours ",MINUTE(SUM($E$4:E69))," minutes"))</f>
         <v/>
+      </c>
+      <c r="I69" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Landing Page Overhaul Done
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70202E76-C491-4E6E-A863-6967E79AB3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB86423D-C321-4872-82B9-CBD79C28E2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="211">
   <si>
     <t>Start Time:</t>
   </si>
@@ -679,6 +679,18 @@
   </si>
   <si>
     <t>I want to get another template or two done, and I want to finish the "try one of these templates" area. I also need to add the project deletion functionality to the frontend</t>
+  </si>
+  <si>
+    <t>I planned out the dashboard rework, and I cleaned up the index and started on the templates panel there</t>
+  </si>
+  <si>
+    <t>Next is to make the template buttons their own component, and crank out the new dashboard</t>
+  </si>
+  <si>
+    <t>I finished the landing page aside from the template buttons for templates that don't exist and template buttons for templates that do exist don't link</t>
+  </si>
+  <si>
+    <t>New Dashboard</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1670,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,11 +2241,11 @@
       </c>
       <c r="BL4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>00 hours 42 minutes</v>
       </c>
       <c r="BM4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 00 minutes</v>
       </c>
       <c r="BN4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -2815,63 +2827,63 @@
       </c>
       <c r="BL6" s="47" t="str" cm="1">
         <f t="array" ref="BL6">INT((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BL$4, 2))), SUM(MID($K$4:BL$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>154 hours 45 minutes</v>
       </c>
       <c r="BM6" s="48" t="str" cm="1">
         <f t="array" ref="BM6">INT((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BM$4, 2))), SUM(MID($K$4:BM$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>154 hours 3 minutes</v>
+        <v>155 hours 45 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4696,27 +4708,57 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E69" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="69" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B69" s="27">
+        <v>45254</v>
+      </c>
+      <c r="C69" s="16">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="D69" s="12">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="E69" s="17">
+        <f t="shared" si="2"/>
+        <v>2.9166666666666674E-2</v>
       </c>
       <c r="F69" s="15" t="str">
         <f>IF(E69="","",_xlfn.CONCAT(HOUR(SUM($E$4:E69))," hours ",MINUTE(SUM($E$4:E69))," minutes"))</f>
-        <v/>
+        <v>10 hours 45 minutes</v>
+      </c>
+      <c r="G69" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="H69" s="25" t="s">
+        <v>208</v>
       </c>
       <c r="I69" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E70" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+    <row r="70" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="27">
+        <v>45255</v>
+      </c>
+      <c r="C70" s="16">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="D70" s="12">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E70" s="17">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="F70" s="15" t="str">
         <f>IF(E70="","",_xlfn.CONCAT(HOUR(SUM($E$4:E70))," hours ",MINUTE(SUM($E$4:E70))," minutes"))</f>
-        <v/>
+        <v>11 hours 45 minutes</v>
+      </c>
+      <c r="G70" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="H70" s="25" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Color tweaks, dashboard progress
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BC64FB-F2C3-4DC4-9315-E4C03FFAA7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B8D948-E8A2-41C2-BD35-1869AD566E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="213">
   <si>
     <t>Start Time:</t>
   </si>
@@ -691,6 +691,12 @@
   </si>
   <si>
     <t>I finished the landing page aside from the template buttons for templates that don't exist and template buttons for templates that do exist don't link. Also made the follower endpoints for the new dashboard</t>
+  </si>
+  <si>
+    <t>A ton of dashboard work as well as tweaks all over. Such as the secondary color now being yellow and projects now store their forks</t>
+  </si>
+  <si>
+    <t>Dashboard project context menu, dashboard following list, public profile overhaul, templates</t>
   </si>
 </sst>
 </file>
@@ -1669,25 +1675,25 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="16" customWidth="1"/>
     <col min="4" max="4" width="10" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="17" customWidth="1"/>
     <col min="6" max="6" width="20" style="15" customWidth="1"/>
-    <col min="7" max="7" width="37.88671875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="21" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" style="51" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:151" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:151" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1701,7 +1707,7 @@
       <c r="H1" s="22"/>
       <c r="J1" s="29"/>
     </row>
-    <row r="2" spans="1:151" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:151" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2"/>
@@ -1749,7 +1755,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:151" s="31" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:151" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
@@ -2002,7 +2008,7 @@
       <c r="ES3" s="41"/>
       <c r="ET3" s="41"/>
     </row>
-    <row r="4" spans="1:151" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:151" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" s="26">
         <v>45201</v>
@@ -2249,7 +2255,7 @@
       </c>
       <c r="BN4" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>04 hours 05 minutes</v>
       </c>
       <c r="BO4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2321,7 +2327,7 @@
       <c r="ES4" s="40"/>
       <c r="ET4" s="42"/>
     </row>
-    <row r="5" spans="1:151" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:151" s="37" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" s="27">
         <v>45202</v>
@@ -2586,7 +2592,7 @@
       <c r="ET5" s="45"/>
       <c r="EU5" s="36"/>
     </row>
-    <row r="6" spans="1:151" s="39" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:151" s="39" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6" s="27">
         <v>45203</v>
@@ -2835,55 +2841,55 @@
       </c>
       <c r="BN6" s="49" t="str" cm="1">
         <f t="array" ref="BN6">INT((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BN$4, 2))), SUM(MID($K$4:BN$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>156 hours 0 minutes</v>
+        <v>160 hours 5 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -2959,7 +2965,7 @@
       <c r="ET6" s="49"/>
       <c r="EU6" s="46"/>
     </row>
-    <row r="7" spans="1:151" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:151" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="27">
         <v>45204</v>
@@ -3159,7 +3165,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:151" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
         <v>45205</v>
       </c>
@@ -3187,7 +3193,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:151" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>45206</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:151" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:151" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>45206</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:151" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:151" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>45207</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:151" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>45207</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:151" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:151" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>45208</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:151" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:151" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>45208</v>
       </c>
@@ -3355,7 +3361,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:151" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:151" ht="120" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>45209</v>
       </c>
@@ -3383,7 +3389,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:151" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:151" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>45209</v>
       </c>
@@ -3408,7 +3414,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>45210</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="27">
         <v>45210</v>
       </c>
@@ -3458,7 +3464,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>45211</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="27">
         <v>45211</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
         <v>45212</v>
       </c>
@@ -3536,7 +3542,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="27">
         <v>45212</v>
       </c>
@@ -3564,7 +3570,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>45213</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>45214</v>
       </c>
@@ -3620,7 +3626,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>45215</v>
       </c>
@@ -3648,7 +3654,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="27">
         <v>45216</v>
       </c>
@@ -3670,7 +3676,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B27" s="27">
         <v>45216</v>
       </c>
@@ -3698,7 +3704,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="27">
         <v>45217</v>
       </c>
@@ -3723,7 +3729,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="27">
         <v>45218</v>
       </c>
@@ -3748,7 +3754,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="27">
         <v>45218</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B31" s="27">
         <v>45218</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="27">
         <v>45219</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="27">
         <v>45220</v>
       </c>
@@ -3845,7 +3851,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="27">
         <v>45220</v>
       </c>
@@ -3898,7 +3904,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="27">
         <v>45221</v>
       </c>
@@ -3923,7 +3929,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="27">
         <v>45221</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" s="27">
         <v>45223</v>
       </c>
@@ -3973,7 +3979,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B39" s="27">
         <v>45224</v>
       </c>
@@ -3998,7 +4004,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="27">
         <v>45225</v>
       </c>
@@ -4020,7 +4026,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B41" s="27">
         <v>45226</v>
       </c>
@@ -4045,7 +4051,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B42" s="27">
         <v>45227</v>
       </c>
@@ -4073,7 +4079,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="27">
         <v>45227</v>
       </c>
@@ -4095,7 +4101,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="27">
         <v>45228</v>
       </c>
@@ -4117,7 +4123,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B45" s="27">
         <v>45228</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="27">
         <v>45230</v>
       </c>
@@ -4164,7 +4170,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B47" s="27">
         <v>45230</v>
       </c>
@@ -4189,7 +4195,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="27">
         <v>45231</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B49" s="27">
         <v>45232</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="27">
         <v>45233</v>
       </c>
@@ -4264,7 +4270,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="27">
         <v>45234</v>
       </c>
@@ -4286,7 +4292,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" s="27">
         <v>45236</v>
       </c>
@@ -4311,7 +4317,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B53" s="27">
         <v>45237</v>
       </c>
@@ -4339,7 +4345,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B54" s="27">
         <v>45238</v>
       </c>
@@ -4364,7 +4370,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B55" s="27">
         <v>45239</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="27">
         <v>45240</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="27">
         <v>45240</v>
       </c>
@@ -4439,7 +4445,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B58" s="27">
         <v>45241</v>
       </c>
@@ -4464,7 +4470,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="27">
         <v>45243</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="27">
         <v>45245</v>
       </c>
@@ -4511,7 +4517,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B61" s="27">
         <v>45245</v>
       </c>
@@ -4536,7 +4542,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B62" s="27">
         <v>45246</v>
       </c>
@@ -4558,7 +4564,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B63" s="27">
         <v>45247</v>
       </c>
@@ -4583,7 +4589,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B64" s="27">
         <v>45248</v>
       </c>
@@ -4608,7 +4614,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B65" s="27">
         <v>45250</v>
       </c>
@@ -4633,7 +4639,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B66" s="27">
         <v>45251</v>
       </c>
@@ -4658,7 +4664,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="27">
         <v>45252</v>
       </c>
@@ -4683,7 +4689,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="27">
         <v>45253</v>
       </c>
@@ -4708,7 +4714,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B69" s="27">
         <v>45254</v>
       </c>
@@ -4736,7 +4742,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B70" s="27">
         <v>45254</v>
       </c>
@@ -4761,17 +4767,32 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E71" s="17" t="str">
+    <row r="71" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B71" s="27">
+        <v>45256</v>
+      </c>
+      <c r="C71" s="16">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D71" s="12">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="E71" s="17">
         <f t="shared" ref="E71:E125" si="3">IF(OR(C71=0, D71=0),"", D71-C71)</f>
-        <v/>
+        <v>0.17013888888888895</v>
       </c>
       <c r="F71" s="15" t="str">
         <f>IF(E71="","",_xlfn.CONCAT(HOUR(SUM($E$4:E71))," hours ",MINUTE(SUM($E$4:E71))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
+        <v>16 hours 5 minutes</v>
+      </c>
+      <c r="G71" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E72" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4781,7 +4802,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E73" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4791,7 +4812,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E74" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4801,7 +4822,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E75" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4811,7 +4832,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E76" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4821,7 +4842,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E77" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4831,7 +4852,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E78" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4841,7 +4862,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E79" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4851,7 +4872,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E80" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4861,7 +4882,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4871,7 +4892,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E82" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4881,7 +4902,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4891,7 +4912,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E84" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4901,7 +4922,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4911,7 +4932,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E86" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4921,7 +4942,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4931,7 +4952,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E88" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4941,7 +4962,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4951,7 +4972,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E90" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4961,7 +4982,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4971,7 +4992,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E92" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4981,7 +5002,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4991,7 +5012,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E94" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5001,7 +5022,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5011,7 +5032,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E96" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5021,7 +5042,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E97" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5031,7 +5052,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E98" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5041,7 +5062,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E99" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5051,7 +5072,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E100" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5061,7 +5082,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E101" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5071,7 +5092,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E102" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5081,7 +5102,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E103" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5091,7 +5112,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E104" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5101,7 +5122,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E105" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5111,121 +5132,121 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E106" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E107" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="108" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E108" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="109" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E109" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="110" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E110" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="111" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E111" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="112" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E112" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>

</xml_diff>

<commit_message>
dashboard work and other tweaks
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B8D948-E8A2-41C2-BD35-1869AD566E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43FE7B3-FBFE-4BEA-9C56-7E5F1145E7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="215">
   <si>
     <t>Start Time:</t>
   </si>
@@ -696,7 +696,13 @@
     <t>A ton of dashboard work as well as tweaks all over. Such as the secondary color now being yellow and projects now store their forks</t>
   </si>
   <si>
-    <t>Dashboard project context menu, dashboard following list, public profile overhaul, templates</t>
+    <t>Dashboard project context menu, dashboard following list, public profile overhaul, templates. ALSO change the edit button on the dashboard to a pencil icon in the corner</t>
+  </si>
+  <si>
+    <t>The following list and the templates</t>
+  </si>
+  <si>
+    <t>Pencil icon and context menus done, started on the following list. Also got the public profile page to be up to date with the dashboard (public profile is just view only dashboard)</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1682,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,7 +2265,7 @@
       </c>
       <c r="BO4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 30 minutes</v>
       </c>
       <c r="BP4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2845,51 +2851,51 @@
       </c>
       <c r="BO6" s="46" t="str" cm="1">
         <f t="array" ref="BO6">INT((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BO$4, 2))), SUM(MID($K$4:BO$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>160 hours 5 minutes</v>
+        <v>162 hours 35 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4767,7 +4773,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="90" x14ac:dyDescent="0.25">
       <c r="B71" s="27">
         <v>45256</v>
       </c>
@@ -4792,14 +4798,29 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E72" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+    <row r="72" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B72" s="27">
+        <v>45257</v>
+      </c>
+      <c r="C72" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="D72" s="12">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E72" s="17">
+        <f t="shared" si="3"/>
+        <v>0.10416666666666663</v>
       </c>
       <c r="F72" s="15" t="str">
         <f>IF(E72="","",_xlfn.CONCAT(HOUR(SUM($E$4:E72))," hours ",MINUTE(SUM($E$4:E72))," minutes"))</f>
-        <v/>
+        <v>18 hours 35 minutes</v>
+      </c>
+      <c r="G72" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="H72" s="25" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Profile following and following display
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43FE7B3-FBFE-4BEA-9C56-7E5F1145E7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD604C3-E223-41F2-A64D-3C99C7BA2C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="224">
   <si>
     <t>Start Time:</t>
   </si>
@@ -703,6 +703,33 @@
   </si>
   <si>
     <t>Pencil icon and context menus done, started on the following list. Also got the public profile page to be up to date with the dashboard (public profile is just view only dashboard)</t>
+  </si>
+  <si>
+    <t>Profile following and following display</t>
+  </si>
+  <si>
+    <t>Get the other templates and their buttons working. Make an endpoint that creates the template files from hard coded values so it's not so difficult</t>
+  </si>
+  <si>
+    <t>162 hours</t>
+  </si>
+  <si>
+    <t>166 hours</t>
+  </si>
+  <si>
+    <t>168 hours</t>
+  </si>
+  <si>
+    <t>170 hours</t>
+  </si>
+  <si>
+    <t>173 hours</t>
+  </si>
+  <si>
+    <t>178 hours</t>
+  </si>
+  <si>
+    <t>180 hours</t>
   </si>
 </sst>
 </file>
@@ -1681,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BV7" sqref="BV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2296,7 @@
       </c>
       <c r="BP4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 45 minutes</v>
       </c>
       <c r="BQ4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2855,47 +2882,47 @@
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>162 hours 35 minutes</v>
+        <v>165 hours 20 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -3170,6 +3197,27 @@
       <c r="BN7" s="39" t="s">
         <v>188</v>
       </c>
+      <c r="BO7" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="BP7" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="BQ7" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="BR7" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="BS7" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="BT7" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="BU7" s="39" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
@@ -4823,14 +4871,29 @@
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E73" s="17" t="str">
+    <row r="73" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B73" s="27">
+        <v>45258</v>
+      </c>
+      <c r="C73" s="16">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D73" s="12">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="E73" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0.11458333333333337</v>
       </c>
       <c r="F73" s="15" t="str">
         <f>IF(E73="","",_xlfn.CONCAT(HOUR(SUM($E$4:E73))," hours ",MINUTE(SUM($E$4:E73))," minutes"))</f>
-        <v/>
+        <v>21 hours 20 minutes</v>
+      </c>
+      <c r="G73" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="H73" s="25" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Project Stuff Templates yaya
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD604C3-E223-41F2-A64D-3C99C7BA2C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B9593A-E6A8-4DCF-8C7E-4DF5D381829F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="226">
   <si>
     <t>Start Time:</t>
   </si>
@@ -730,6 +730,12 @@
   </si>
   <si>
     <t>180 hours</t>
+  </si>
+  <si>
+    <t>More Template stuff</t>
+  </si>
+  <si>
+    <t>More Template Stuff, finalize the web trio template</t>
   </si>
 </sst>
 </file>
@@ -1708,8 +1714,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BV7" sqref="BV7"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BQ10" sqref="BQ10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,7 +2302,7 @@
       </c>
       <c r="BP4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>02 hours 45 minutes</v>
+        <v>04 hours 50 minutes</v>
       </c>
       <c r="BQ4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2882,47 +2888,47 @@
       </c>
       <c r="BP6" s="37" t="str" cm="1">
         <f t="array" ref="BP6">INT((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BP$4, 2))), SUM(MID($K$4:BP$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>165 hours 20 minutes</v>
+        <v>167 hours 25 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4896,14 +4902,29 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E74" s="17" t="str">
+    <row r="74" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B74" s="27">
+        <v>45258</v>
+      </c>
+      <c r="C74" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="D74" s="12">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="E74" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>8.6805555555555469E-2</v>
       </c>
       <c r="F74" s="15" t="str">
         <f>IF(E74="","",_xlfn.CONCAT(HOUR(SUM($E$4:E74))," hours ",MINUTE(SUM($E$4:E74))," minutes"))</f>
-        <v/>
+        <v>23 hours 25 minutes</v>
+      </c>
+      <c r="G74" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H74" s="25" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small tweaks from usage
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B9593A-E6A8-4DCF-8C7E-4DF5D381829F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFAD6B6-8D0D-462C-8E09-8444B8BF2621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="229">
   <si>
     <t>Start Time:</t>
   </si>
@@ -736,6 +736,15 @@
   </si>
   <si>
     <t>More Template Stuff, finalize the web trio template</t>
+  </si>
+  <si>
+    <t>All the templates are made</t>
+  </si>
+  <si>
+    <t>also start testing everything you can think of and figure out what to show off when</t>
+  </si>
+  <si>
+    <t>Next I need to make a method that will manually insert these templates into the database from hard coded versions so I don't lose the templates. Also connect the templates to the buttons, maybe just allow the ID to be an int? let hard coded IDs be these?</t>
   </si>
 </sst>
 </file>
@@ -1714,8 +1723,8 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BQ10" sqref="BQ10"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,7 +2315,7 @@
       </c>
       <c r="BQ4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 15 minutes</v>
       </c>
       <c r="BR4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2892,43 +2901,43 @@
       </c>
       <c r="BQ6" s="37" t="str" cm="1">
         <f t="array" ref="BQ6">INT((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BQ$4, 2))), SUM(MID($K$4:BQ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>167 hours 25 minutes</v>
+        <v>169 hours 40 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4927,14 +4936,32 @@
         <v>225</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E75" s="17" t="str">
+    <row r="75" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="B75" s="27">
+        <v>45259</v>
+      </c>
+      <c r="C75" s="16">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="D75" s="12">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E75" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>9.375E-2</v>
       </c>
       <c r="F75" s="15" t="str">
         <f>IF(E75="","",_xlfn.CONCAT(HOUR(SUM($E$4:E75))," hours ",MINUTE(SUM($E$4:E75))," minutes"))</f>
-        <v/>
+        <v>1 hours 40 minutes</v>
+      </c>
+      <c r="G75" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="I75" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Templates are tied to their buttons
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C939E09-043E-47FC-A4F8-019E4C0126F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740135A-DDDB-484A-9A1C-40259E2847BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="233">
   <si>
     <t>Start Time:</t>
   </si>
@@ -745,6 +745,18 @@
   </si>
   <si>
     <t>Next I need to make a method that will manually insert these templates into the database from hard coded versions so I don't lose the templates. Also connect the templates to the buttons, maybe just allow the ID to be an int? let hard coded IDs be these?</t>
+  </si>
+  <si>
+    <t>Did the things I said I need to, templates can be easily initialized, and the buttons point to the templates</t>
+  </si>
+  <si>
+    <t>Write my presentation outline and start on the slides. Also try getting webbie on fly.io</t>
+  </si>
+  <si>
+    <t>https://fly.io/docs/languages-and-frameworks/dockerfile/</t>
+  </si>
+  <si>
+    <t>https://chat.openai.com/g/g-lN1gKFnvL-creative-writing-coach/c/2fa968c8-68f9-4f26-a586-747bc7f4e439</t>
   </si>
 </sst>
 </file>
@@ -1302,7 +1314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1395,6 +1407,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1724,7 +1737,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2332,7 @@
       </c>
       <c r="BR4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>01 hours 30 minutes</v>
+        <v>02 hours 50 minutes</v>
       </c>
       <c r="BS4" s="35" t="str">
         <f t="shared" si="1"/>
@@ -2905,39 +2918,39 @@
       </c>
       <c r="BR6" s="37" t="str" cm="1">
         <f t="array" ref="BR6">INT((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BR$4, 2))), SUM(MID($K$4:BR$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>171 hours 10 minutes</v>
+        <v>172 hours 30 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -4683,7 +4696,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B65" s="27">
         <v>45250</v>
       </c>
@@ -4708,7 +4721,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12" ht="60" x14ac:dyDescent="0.25">
       <c r="B66" s="27">
         <v>45251</v>
       </c>
@@ -4733,7 +4746,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="27">
         <v>45252</v>
       </c>
@@ -4758,7 +4771,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="27">
         <v>45253</v>
       </c>
@@ -4783,7 +4796,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B69" s="27">
         <v>45254</v>
       </c>
@@ -4811,7 +4824,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B70" s="27">
         <v>45254</v>
       </c>
@@ -4836,7 +4849,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="71" spans="2:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" ht="90" x14ac:dyDescent="0.25">
       <c r="B71" s="27">
         <v>45256</v>
       </c>
@@ -4861,7 +4874,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B72" s="27">
         <v>45257</v>
       </c>
@@ -4886,7 +4899,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B73" s="27">
         <v>45258</v>
       </c>
@@ -4911,7 +4924,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="74" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="27">
         <v>45258</v>
       </c>
@@ -4936,7 +4949,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="75" spans="2:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" ht="105" x14ac:dyDescent="0.25">
       <c r="B75" s="27">
         <v>45259</v>
       </c>
@@ -4964,7 +4977,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="27">
         <v>45260</v>
       </c>
@@ -4972,18 +4985,30 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="D76" s="12">
-        <v>0.61805555555555558</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="E76" s="17">
         <f t="shared" si="3"/>
-        <v>6.25E-2</v>
+        <v>0.11805555555555558</v>
       </c>
       <c r="F76" s="15" t="str">
         <f>IF(E76="","",_xlfn.CONCAT(HOUR(SUM($E$4:E76))," hours ",MINUTE(SUM($E$4:E76))," minutes"))</f>
-        <v>3 hours 10 minutes</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+        <v>4 hours 30 minutes</v>
+      </c>
+      <c r="G76" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="I76" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="L76" s="54" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E77" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -4993,7 +5018,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E78" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5003,7 +5028,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E79" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5013,7 +5038,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E80" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5398,9 +5423,11 @@
   <hyperlinks>
     <hyperlink ref="H13" r:id="rId1" xr:uid="{40BF5D3F-6F40-4D36-A2D2-A18CA464B327}"/>
     <hyperlink ref="J27" r:id="rId2" xr:uid="{9F3B3340-4F24-4554-BB1A-2EA07283D5A7}"/>
+    <hyperlink ref="I76" r:id="rId3" xr:uid="{195CE167-8226-445C-BA43-7F3E1C527220}"/>
+    <hyperlink ref="L76" r:id="rId4" xr:uid="{067E891A-7FE5-40AC-9173-27376CAA17E9}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First capstone rehearsal patch Fixed some bugs from rehearsal
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740135A-DDDB-484A-9A1C-40259E2847BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933761FE-7CBD-4D30-AAD4-ED94BCAB01ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="235">
   <si>
     <t>Start Time:</t>
   </si>
@@ -757,6 +757,12 @@
   </si>
   <si>
     <t>https://chat.openai.com/g/g-lN1gKFnvL-creative-writing-coach/c/2fa968c8-68f9-4f26-a586-747bc7f4e439</t>
+  </si>
+  <si>
+    <t>Presentation Outline</t>
+  </si>
+  <si>
+    <t>Test production build of frontend, get hosted on fly.io, practice runs of presentation, backup recording</t>
   </si>
 </sst>
 </file>
@@ -1737,7 +1743,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,7 +2342,7 @@
       </c>
       <c r="BS4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>02 hours 00 minutes</v>
       </c>
       <c r="BT4" s="40" t="str">
         <f t="shared" si="1"/>
@@ -2922,35 +2928,35 @@
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BV6" s="46" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BW6" s="37" t="str" cm="1">
         <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BX6" s="37" t="str" cm="1">
         <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BY6" s="37" t="str" cm="1">
         <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="BZ6" s="47" t="str" cm="1">
         <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>172 hours 30 minutes</v>
+        <v>174 hours 30 minutes</v>
       </c>
       <c r="CA6" s="48"/>
       <c r="CB6" s="49"/>
@@ -5008,14 +5014,29 @@
         <v>232</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E77" s="17" t="str">
+    <row r="77" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B77" s="27">
+        <v>45261</v>
+      </c>
+      <c r="C77" s="16">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="D77" s="12">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E77" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="F77" s="15" t="str">
         <f>IF(E77="","",_xlfn.CONCAT(HOUR(SUM($E$4:E77))," hours ",MINUTE(SUM($E$4:E77))," minutes"))</f>
-        <v/>
+        <v>6 hours 30 minutes</v>
+      </c>
+      <c r="G77" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="H77" s="25" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Untested, but likely final build
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933761FE-7CBD-4D30-AAD4-ED94BCAB01ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196320B9-CCB0-4D0A-BBA1-B25E0A0D18AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
+    <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="239">
   <si>
     <t>Start Time:</t>
   </si>
@@ -763,6 +763,18 @@
   </si>
   <si>
     <t>Test production build of frontend, get hosted on fly.io, practice runs of presentation, backup recording</t>
+  </si>
+  <si>
+    <t>Started fixing ESLint quality issues getting in the way of a production build of next</t>
+  </si>
+  <si>
+    <t>Finish up getting a production build of next.js going, also record a backup presentation</t>
+  </si>
+  <si>
+    <t>Production build is made</t>
+  </si>
+  <si>
+    <t>Test production build and do a rehearsal run</t>
   </si>
 </sst>
 </file>
@@ -819,7 +831,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -880,8 +892,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1315,12 +1339,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.79998168889431442"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.79995117038483843"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCFF"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1414,6 +1495,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1742,7 +1838,7 @@
   </sheetPr>
   <dimension ref="A1:EU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
@@ -2038,21 +2134,13 @@
       <c r="BU3" s="41">
         <v>45263</v>
       </c>
-      <c r="BV3" s="31">
+      <c r="BV3" s="65">
         <v>45264</v>
       </c>
-      <c r="BW3" s="31">
-        <v>45265</v>
-      </c>
-      <c r="BX3" s="31">
-        <v>45266</v>
-      </c>
-      <c r="BY3" s="31">
-        <v>45267</v>
-      </c>
-      <c r="BZ3" s="31">
-        <v>45268</v>
-      </c>
+      <c r="BW3" s="59"/>
+      <c r="BX3" s="59"/>
+      <c r="BY3" s="59"/>
+      <c r="BZ3" s="59"/>
       <c r="CA3" s="41"/>
       <c r="CB3" s="41"/>
       <c r="CH3" s="41"/>
@@ -2193,7 +2281,7 @@
         <v>04 hours 17 minutes</v>
       </c>
       <c r="AH4" s="35" t="str">
-        <f t="shared" ref="AH4:BZ4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AH$3), "hh ""hours ""mm ""minutes""")</f>
+        <f t="shared" ref="AH4:BV4" si="1">TEXT(SUMIFS($E$3:$E$99, $B$3:$B$99, AH$3), "hh ""hours ""mm ""minutes""")</f>
         <v>02 hours 08 minutes</v>
       </c>
       <c r="AI4" s="35" t="str">
@@ -2342,37 +2430,25 @@
       </c>
       <c r="BS4" s="35" t="str">
         <f t="shared" si="1"/>
-        <v>02 hours 00 minutes</v>
+        <v>02 hours 27 minutes</v>
       </c>
       <c r="BT4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>01 hours 55 minutes</v>
       </c>
       <c r="BU4" s="42" t="str">
         <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BV4" s="35" t="str">
+      <c r="BV4" s="61" t="str">
         <f t="shared" si="1"/>
         <v>00 hours 00 minutes</v>
       </c>
-      <c r="BW4" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
-      </c>
-      <c r="BX4" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
-      </c>
-      <c r="BY4" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
-      </c>
-      <c r="BZ4" s="35" t="str">
-        <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
-      </c>
-      <c r="CA4" s="40"/>
+      <c r="BW4" s="60"/>
+      <c r="BX4" s="60"/>
+      <c r="BY4" s="60"/>
+      <c r="BZ4" s="60"/>
+      <c r="CA4" s="55"/>
       <c r="CB4" s="42"/>
       <c r="CH4" s="40"/>
       <c r="CI4" s="42"/>
@@ -2610,22 +2686,14 @@
       <c r="BU5" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="BV5" s="36" t="s">
+      <c r="BV5" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="BW5" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="BX5" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="BY5" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="BZ5" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="CA5" s="44"/>
+      <c r="BW5" s="60"/>
+      <c r="BX5" s="60"/>
+      <c r="BY5" s="60"/>
+      <c r="BZ5" s="60"/>
+      <c r="CA5" s="56"/>
       <c r="CB5" s="45"/>
       <c r="CC5" s="36"/>
       <c r="CH5" s="44"/>
@@ -2928,37 +2996,25 @@
       </c>
       <c r="BS6" s="47" t="str" cm="1">
         <f t="array" ref="BS6">INT((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BS$4, 2))), SUM(MID($K$4:BS$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
+        <v>174 hours 57 minutes</v>
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
+        <v>176 hours 52 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="BV6" s="46" t="str" cm="1">
+        <v>176 hours 52 minutes</v>
+      </c>
+      <c r="BV6" s="63" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="BW6" s="37" t="str" cm="1">
-        <f t="array" ref="BW6">INT((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BW$4, 2))), SUM(MID($K$4:BW$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="BX6" s="37" t="str" cm="1">
-        <f t="array" ref="BX6">INT((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BX$4, 2))), SUM(MID($K$4:BX$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="BY6" s="37" t="str" cm="1">
-        <f t="array" ref="BY6">INT((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BY$4, 2))), SUM(MID($K$4:BY$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="BZ6" s="47" t="str" cm="1">
-        <f t="array" ref="BZ6">INT((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BZ$4, 2))), SUM(MID($K$4:BZ$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>174 hours 30 minutes</v>
-      </c>
-      <c r="CA6" s="48"/>
+        <v>176 hours 52 minutes</v>
+      </c>
+      <c r="BW6" s="60"/>
+      <c r="BX6" s="60"/>
+      <c r="BY6" s="60"/>
+      <c r="BZ6" s="60"/>
+      <c r="CA6" s="57"/>
       <c r="CB6" s="49"/>
       <c r="CC6" s="46"/>
       <c r="CD6" s="37"/>
@@ -3252,6 +3308,12 @@
       <c r="BU7" s="39" t="s">
         <v>223</v>
       </c>
+      <c r="BV7" s="64"/>
+      <c r="BW7" s="59"/>
+      <c r="BX7" s="59"/>
+      <c r="BY7" s="59"/>
+      <c r="BZ7" s="59"/>
+      <c r="CA7" s="58"/>
     </row>
     <row r="8" spans="1:151" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
@@ -5039,24 +5101,54 @@
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E78" s="17" t="str">
+    <row r="78" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="27">
+        <v>45261</v>
+      </c>
+      <c r="C78" s="16">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D78" s="12">
+        <v>0.7895833333333333</v>
+      </c>
+      <c r="E78" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1.8749999999999933E-2</v>
       </c>
       <c r="F78" s="15" t="str">
         <f>IF(E78="","",_xlfn.CONCAT(HOUR(SUM($E$4:E78))," hours ",MINUTE(SUM($E$4:E78))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E79" s="17" t="str">
+        <v>6 hours 57 minutes</v>
+      </c>
+      <c r="G78" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="H78" s="25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="27">
+        <v>45262</v>
+      </c>
+      <c r="C79" s="16">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D79" s="12">
+        <v>0.59375</v>
+      </c>
+      <c r="E79" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>7.9861111111111049E-2</v>
       </c>
       <c r="F79" s="15" t="str">
         <f>IF(E79="","",_xlfn.CONCAT(HOUR(SUM($E$4:E79))," hours ",MINUTE(SUM($E$4:E79))," minutes"))</f>
-        <v/>
+        <v>8 hours 52 minutes</v>
+      </c>
+      <c r="G79" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="H79" s="25" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Deleted a whole API last minute
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196320B9-CCB0-4D0A-BBA1-B25E0A0D18AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64529896-C2A3-4ABA-93B4-B28BBBE5A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="241">
   <si>
     <t>Start Time:</t>
   </si>
@@ -775,6 +775,12 @@
   </si>
   <si>
     <t>Test production build and do a rehearsal run</t>
+  </si>
+  <si>
+    <t>Dockerized entirely!</t>
+  </si>
+  <si>
+    <t>Practice Practice!</t>
   </si>
 </sst>
 </file>
@@ -1839,7 +1845,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2434,7 +2440,7 @@
       </c>
       <c r="BT4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>01 hours 55 minutes</v>
+        <v>02 hours 50 minutes</v>
       </c>
       <c r="BU4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -3000,15 +3006,15 @@
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>176 hours 52 minutes</v>
+        <v>177 hours 47 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>176 hours 52 minutes</v>
+        <v>177 hours 47 minutes</v>
       </c>
       <c r="BV6" s="63" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>176 hours 52 minutes</v>
+        <v>177 hours 47 minutes</v>
       </c>
       <c r="BW6" s="60"/>
       <c r="BX6" s="60"/>
@@ -5152,13 +5158,28 @@
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E80" s="17" t="str">
+      <c r="B80" s="27">
+        <v>45262</v>
+      </c>
+      <c r="C80" s="16">
+        <v>0.71180555555555547</v>
+      </c>
+      <c r="D80" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="E80" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.8194444444444531E-2</v>
       </c>
       <c r="F80" s="15" t="str">
         <f>IF(E80="","",_xlfn.CONCAT(HOUR(SUM($E$4:E80))," hours ",MINUTE(SUM($E$4:E80))," minutes"))</f>
-        <v/>
+        <v>9 hours 47 minutes</v>
+      </c>
+      <c r="G80" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" s="25" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Did some runs and fixed some bugs + polish
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64529896-C2A3-4ABA-93B4-B28BBBE5A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC5733F-602D-46AF-AFBA-C9DB86C4F71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5232" windowWidth="23256" windowHeight="14016" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="242">
   <si>
     <t>Start Time:</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>Practice Practice!</t>
+  </si>
+  <si>
+    <t>Testing and Tweaks because practice runs</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1848,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H81" sqref="H81"/>
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,7 +2443,7 @@
       </c>
       <c r="BT4" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>02 hours 50 minutes</v>
+        <v>03 hours 40 minutes</v>
       </c>
       <c r="BU4" s="42" t="str">
         <f t="shared" si="1"/>
@@ -3006,15 +3009,15 @@
       </c>
       <c r="BT6" s="48" t="str" cm="1">
         <f t="array" ref="BT6">INT((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BT$4, 2))), SUM(MID($K$4:BT$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>177 hours 47 minutes</v>
+        <v>178 hours 37 minutes</v>
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>177 hours 47 minutes</v>
+        <v>178 hours 37 minutes</v>
       </c>
       <c r="BV6" s="63" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>177 hours 47 minutes</v>
+        <v>178 hours 37 minutes</v>
       </c>
       <c r="BW6" s="60"/>
       <c r="BX6" s="60"/>
@@ -5182,17 +5185,29 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E81" s="17" t="str">
+    <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="27">
+        <v>45262</v>
+      </c>
+      <c r="C81" s="16">
+        <v>0.8125</v>
+      </c>
+      <c r="D81" s="12">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E81" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="F81" s="15" t="str">
         <f>IF(E81="","",_xlfn.CONCAT(HOUR(SUM($E$4:E81))," hours ",MINUTE(SUM($E$4:E81))," minutes"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+        <v>10 hours 37 minutes</v>
+      </c>
+      <c r="G81" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E82" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5202,7 +5217,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E83" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5212,7 +5227,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E84" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5222,7 +5237,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E85" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5232,7 +5247,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E86" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5242,7 +5257,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E87" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5252,7 +5267,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E88" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5262,7 +5277,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E89" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5272,7 +5287,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E90" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5282,7 +5297,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E91" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5292,7 +5307,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E92" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5302,7 +5317,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E93" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5312,7 +5327,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E94" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5322,7 +5337,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E95" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5332,7 +5347,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="E96" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>

</xml_diff>

<commit_message>
Last Hour Tracker Update
</commit_message>
<xml_diff>
--- a/Documents/Capstone Hour Tracker.xlsx
+++ b/Documents/Capstone Hour Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbates\Documents\School Docs\Capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD56EF3-8773-4C85-A658-737F7EBFA07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7078F58-D6D4-4423-9617-98C0AAC6ACBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-6495" windowWidth="19440" windowHeight="11640" xr2:uid="{FFC61897-BE93-43E3-B722-FE8F6A604BE5}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="244">
   <si>
     <t>Start Time:</t>
   </si>
@@ -786,7 +786,10 @@
     <t>Testing and Tweaks because practice runs</t>
   </si>
   <si>
-    <t>IT'S HOSTED YEAAAAAAAAAAAAHH</t>
+    <t>IT'S HOSTED YEAAAAAAAAAAAAHH, also recorded the backup vid and fixed some more small issues</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
 </sst>
 </file>
@@ -1851,7 +1854,7 @@
   <dimension ref="A1:EU125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,7 +2453,7 @@
       </c>
       <c r="BU4" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>00 hours 00 minutes</v>
+        <v>05 hours 45 minutes</v>
       </c>
       <c r="BV4" s="61" t="str">
         <f t="shared" si="1"/>
@@ -3016,11 +3019,11 @@
       </c>
       <c r="BU6" s="49" t="str" cm="1">
         <f t="array" ref="BU6">INT((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BU$4, 2))), SUM(MID($K$4:BU$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>178 hours 37 minutes</v>
+        <v>184 hours 22 minutes</v>
       </c>
       <c r="BV6" s="63" t="str" cm="1">
         <f t="array" ref="BV6">INT((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60)))) &amp; " hours " &amp; MOD((SUM(SUM(INT(LEFT($K$4:BV$4, 2))), SUM(MID($K$4:BV$4,10,2)/60))) * 60, 60) &amp; " minutes"</f>
-        <v>178 hours 37 minutes</v>
+        <v>184 hours 22 minutes</v>
       </c>
       <c r="BW6" s="60"/>
       <c r="BX6" s="60"/>
@@ -5188,7 +5191,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="81" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="27">
         <v>45262</v>
       </c>
@@ -5210,27 +5213,32 @@
         <v>241</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B82" s="27">
         <v>45263</v>
       </c>
       <c r="C82" s="16">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="17" t="str">
+      <c r="D82" s="12">
+        <v>0.9375</v>
+      </c>
+      <c r="E82" s="17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0.23958333333333337</v>
       </c>
       <c r="F82" s="15" t="str">
         <f>IF(E82="","",_xlfn.CONCAT(HOUR(SUM($E$4:E82))," hours ",MINUTE(SUM($E$4:E82))," minutes"))</f>
-        <v/>
+        <v>16 hours 22 minutes</v>
       </c>
       <c r="G82" s="21" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E83" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5240,7 +5248,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E84" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5250,7 +5258,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E85" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5260,7 +5268,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E86" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5270,7 +5278,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E87" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5280,7 +5288,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E88" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5290,7 +5298,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E89" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5300,7 +5308,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E90" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5310,7 +5318,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E91" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5320,7 +5328,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E92" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5330,7 +5338,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E93" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5340,7 +5348,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E94" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5350,7 +5358,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E95" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5360,7 +5368,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E96" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>

</xml_diff>